<commit_message>
finished generating simplex airfoils
</commit_message>
<xml_diff>
--- a/mmtime/data/wart-flights.xlsx
+++ b/mmtime/data/wart-flights.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rblack/_dev/nffs-symposium/live-2022/mmtime/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{231C7C22-8F48-0F49-85AC-618F42120BC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAAB06F4-F77C-004C-9D00-EF6BDE988D1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7640" yWindow="1480" windowWidth="28140" windowHeight="17440" xr2:uid="{6F3648B4-9E08-B641-B142-5EC1E81BAFE5}"/>
+    <workbookView xWindow="5460" yWindow="1480" windowWidth="28140" windowHeight="17440" xr2:uid="{6F3648B4-9E08-B641-B142-5EC1E81BAFE5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>weight</t>
   </si>
@@ -120,17 +120,29 @@
   <si>
     <t>Navg/Q</t>
   </si>
+  <si>
+    <t>Ozanam</t>
+  </si>
+  <si>
+    <t>Oswatomie</t>
+  </si>
+  <si>
+    <t>KC Bible College</t>
+  </si>
+  <si>
+    <t>Westport</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="166" formatCode="0.0"/>
-    <numFmt numFmtId="169" formatCode="0.0000"/>
-    <numFmt numFmtId="170" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -141,6 +153,22 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -166,14 +194,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1504,10 +1536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09968BF9-8E55-D94B-BD5A-1085DDB7CB2E}">
-  <dimension ref="A1:AA34"/>
+  <dimension ref="A1:AA83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U2" sqref="U2"/>
+      <selection activeCell="X83" sqref="X83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1516,7 +1548,8 @@
     <col min="2" max="2" width="11.5" customWidth="1"/>
     <col min="3" max="3" width="5.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6.5" customWidth="1"/>
     <col min="9" max="9" width="5.33203125" bestFit="1" customWidth="1"/>
@@ -1528,11 +1561,11 @@
     <col min="15" max="15" width="5.33203125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="6.6640625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.6640625" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="7" bestFit="1" customWidth="1"/>
     <col min="24" max="25" width="5.6640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -2015,7 +2048,7 @@
         <v>0.5873930504627205</v>
       </c>
       <c r="U9" s="5">
-        <f t="shared" ref="U7:U35" si="8">D9/(1.2+D9)</f>
+        <f t="shared" ref="U9:U34" si="8">D9/(1.2+D9)</f>
         <v>0.40886699507389163</v>
       </c>
       <c r="V9" s="1">
@@ -2039,7 +2072,7 @@
         <v>0.15595959595959596</v>
       </c>
       <c r="AA9">
-        <f t="shared" ref="AA9:AA15" si="14">O9/K9</f>
+        <f t="shared" ref="AA9:AA12" si="14">O9/K9</f>
         <v>2.1931818181818183</v>
       </c>
     </row>
@@ -2586,7 +2619,7 @@
         <v>0.43127962085308064</v>
       </c>
       <c r="V18" s="1">
-        <f t="shared" ref="V18:V26" si="19">6.61 * D18</f>
+        <f t="shared" ref="V18:V21" si="19">6.61 * D18</f>
         <v>6.0151000000000003</v>
       </c>
       <c r="W18" s="3">
@@ -3369,7 +3402,7 @@
         <v>7.3869346733668344</v>
       </c>
       <c r="P30">
-        <f t="shared" ref="P30:P32" si="34">G30*H30</f>
+        <f t="shared" ref="P30:P34" si="34">G30*H30</f>
         <v>29172</v>
       </c>
       <c r="Q30" s="2"/>
@@ -3434,15 +3467,15 @@
         <v>23680</v>
       </c>
       <c r="Q31" s="2">
-        <f t="shared" ref="Q30:Q32" si="35">P31/D31</f>
+        <f t="shared" ref="Q31:Q34" si="35">P31/D31</f>
         <v>32000</v>
       </c>
       <c r="R31" s="5">
-        <f t="shared" ref="R31:R32" si="36">P31/I31</f>
+        <f t="shared" ref="R31:R34" si="36">P31/I31</f>
         <v>7.7008130081300816</v>
       </c>
       <c r="S31" s="4">
-        <f t="shared" ref="S31:S32" si="37">R31/I31</f>
+        <f t="shared" ref="S31:S34" si="37">R31/I31</f>
         <v>2.5043294335382379E-3</v>
       </c>
       <c r="T31" s="5">
@@ -3599,6 +3632,9 @@
         <f t="shared" si="33"/>
         <v>0</v>
       </c>
+      <c r="Q33" s="2"/>
+      <c r="R33" s="5"/>
+      <c r="S33" s="4"/>
       <c r="T33" s="5">
         <f t="shared" si="44"/>
         <v>0.12416911844829466</v>
@@ -3658,6 +3694,22 @@
         <f t="shared" si="33"/>
         <v>7.5</v>
       </c>
+      <c r="P34">
+        <f t="shared" si="34"/>
+        <v>0</v>
+      </c>
+      <c r="Q34" s="2">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="R34" s="5">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="S34" s="4">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
       <c r="T34" s="5">
         <f t="shared" si="44"/>
         <v>0.13324460218870157</v>
@@ -3689,6 +3741,3841 @@
       <c r="AA34">
         <f t="shared" si="43"/>
         <v>2.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>28</v>
+      </c>
+      <c r="B36" s="7">
+        <v>17.5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A37" s="8">
+        <v>40259</v>
+      </c>
+      <c r="C37">
+        <v>47</v>
+      </c>
+      <c r="D37">
+        <v>0.33</v>
+      </c>
+      <c r="E37">
+        <v>30</v>
+      </c>
+      <c r="F37">
+        <v>40</v>
+      </c>
+      <c r="G37">
+        <f t="shared" ref="G37:G55" si="45">E37*F37</f>
+        <v>1200</v>
+      </c>
+      <c r="H37">
+        <v>9</v>
+      </c>
+      <c r="I37">
+        <v>1500</v>
+      </c>
+      <c r="J37" s="2">
+        <f t="shared" ref="J37:J60" si="46">I37/H37</f>
+        <v>166.66666666666666</v>
+      </c>
+      <c r="K37">
+        <v>0.6</v>
+      </c>
+      <c r="L37" s="3">
+        <v>4</v>
+      </c>
+      <c r="M37">
+        <v>18</v>
+      </c>
+      <c r="N37">
+        <f t="shared" ref="N37:N42" si="47">L37*60+M37</f>
+        <v>258</v>
+      </c>
+      <c r="O37" s="1">
+        <f t="shared" ref="O37:O42" si="48">I37/N37</f>
+        <v>5.8139534883720927</v>
+      </c>
+      <c r="P37">
+        <f t="shared" ref="P37:P55" si="49">G37*H37</f>
+        <v>10800</v>
+      </c>
+      <c r="Q37" s="2">
+        <f t="shared" ref="Q37:Q55" si="50">P37/D37</f>
+        <v>32727.272727272724</v>
+      </c>
+      <c r="R37" s="5">
+        <f t="shared" ref="R37:R55" si="51">P37/I37</f>
+        <v>7.2</v>
+      </c>
+      <c r="S37" s="4">
+        <f t="shared" ref="S37:S55" si="52">R37/I37</f>
+        <v>4.8000000000000004E-3</v>
+      </c>
+      <c r="T37" s="5">
+        <f>$B$36/(483*U37)</f>
+        <v>0.16798418972332013</v>
+      </c>
+      <c r="U37" s="5">
+        <f t="shared" ref="U37:U60" si="53">D37/(1.2+D37)</f>
+        <v>0.21568627450980393</v>
+      </c>
+      <c r="V37" s="1">
+        <f t="shared" ref="V37:V60" si="54">6.61 * D37</f>
+        <v>2.1813000000000002</v>
+      </c>
+      <c r="W37" s="3">
+        <f t="shared" ref="W37:W60" si="55">45.257*H37/SQRT(D37/H37)</f>
+        <v>2127.1227684084943</v>
+      </c>
+      <c r="X37" s="5">
+        <f t="shared" ref="X37:X60" si="56">I37/W37</f>
+        <v>0.70517791557574028</v>
+      </c>
+      <c r="Y37" s="5">
+        <f t="shared" ref="Y37:Y42" si="57">N37/J37</f>
+        <v>1.548</v>
+      </c>
+      <c r="Z37">
+        <f t="shared" ref="Z37:Z42" si="58">O37/C37</f>
+        <v>0.12370113805047006</v>
+      </c>
+      <c r="AA37">
+        <f t="shared" ref="AA37:AA42" si="59">O37/K37</f>
+        <v>9.6899224806201545</v>
+      </c>
+    </row>
+    <row r="38" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A38" s="8">
+        <v>38429</v>
+      </c>
+      <c r="C38">
+        <v>45</v>
+      </c>
+      <c r="D38" s="10">
+        <v>0.61</v>
+      </c>
+      <c r="E38" s="7">
+        <v>30</v>
+      </c>
+      <c r="F38" s="10">
+        <v>42</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="45"/>
+        <v>1260</v>
+      </c>
+      <c r="H38">
+        <v>14.5</v>
+      </c>
+      <c r="I38" s="7">
+        <v>1675</v>
+      </c>
+      <c r="J38" s="2">
+        <f t="shared" si="46"/>
+        <v>115.51724137931035</v>
+      </c>
+      <c r="K38" s="10">
+        <v>0.4</v>
+      </c>
+      <c r="L38" s="3">
+        <v>3</v>
+      </c>
+      <c r="M38" s="10">
+        <v>58</v>
+      </c>
+      <c r="N38">
+        <f t="shared" si="47"/>
+        <v>238</v>
+      </c>
+      <c r="O38" s="1">
+        <f t="shared" si="48"/>
+        <v>7.03781512605042</v>
+      </c>
+      <c r="P38">
+        <f t="shared" si="49"/>
+        <v>18270</v>
+      </c>
+      <c r="Q38" s="2">
+        <f t="shared" si="50"/>
+        <v>29950.819672131147</v>
+      </c>
+      <c r="R38" s="5">
+        <f t="shared" si="51"/>
+        <v>10.907462686567165</v>
+      </c>
+      <c r="S38" s="4">
+        <f t="shared" si="52"/>
+        <v>6.511918021831143E-3</v>
+      </c>
+      <c r="T38" s="5">
+        <f t="shared" ref="T38:T60" si="60">$B$36/(483*U38)</f>
+        <v>0.10750772154906153</v>
+      </c>
+      <c r="U38" s="5">
+        <f t="shared" si="53"/>
+        <v>0.33701657458563533</v>
+      </c>
+      <c r="V38" s="1">
+        <f t="shared" si="54"/>
+        <v>4.0320999999999998</v>
+      </c>
+      <c r="W38" s="3">
+        <f t="shared" si="55"/>
+        <v>3199.4317322992915</v>
+      </c>
+      <c r="X38" s="5">
+        <f t="shared" si="56"/>
+        <v>0.52353047045521761</v>
+      </c>
+      <c r="Y38" s="5">
+        <f t="shared" si="57"/>
+        <v>2.0602985074626865</v>
+      </c>
+      <c r="Z38">
+        <f t="shared" si="58"/>
+        <v>0.15639589169000934</v>
+      </c>
+      <c r="AA38">
+        <f t="shared" si="59"/>
+        <v>17.594537815126049</v>
+      </c>
+    </row>
+    <row r="39" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A39" s="8">
+        <v>39922</v>
+      </c>
+      <c r="C39">
+        <v>47</v>
+      </c>
+      <c r="D39" s="9">
+        <v>0.77</v>
+      </c>
+      <c r="E39">
+        <v>44</v>
+      </c>
+      <c r="F39">
+        <v>40</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="45"/>
+        <v>1760</v>
+      </c>
+      <c r="H39">
+        <v>15.25</v>
+      </c>
+      <c r="I39">
+        <v>1825</v>
+      </c>
+      <c r="J39" s="2">
+        <f t="shared" si="46"/>
+        <v>119.67213114754098</v>
+      </c>
+      <c r="K39" s="10">
+        <v>0.59</v>
+      </c>
+      <c r="L39" s="3">
+        <v>4</v>
+      </c>
+      <c r="M39" s="10">
+        <v>1</v>
+      </c>
+      <c r="N39">
+        <f t="shared" si="47"/>
+        <v>241</v>
+      </c>
+      <c r="O39" s="1">
+        <f t="shared" si="48"/>
+        <v>7.5726141078838172</v>
+      </c>
+      <c r="P39">
+        <f t="shared" si="49"/>
+        <v>26840</v>
+      </c>
+      <c r="Q39" s="2">
+        <f t="shared" si="50"/>
+        <v>34857.142857142855</v>
+      </c>
+      <c r="R39" s="5">
+        <f t="shared" si="51"/>
+        <v>14.706849315068494</v>
+      </c>
+      <c r="S39" s="4">
+        <f t="shared" si="52"/>
+        <v>8.0585475699005444E-3</v>
+      </c>
+      <c r="T39" s="5">
+        <f t="shared" si="60"/>
+        <v>9.2697157914549216E-2</v>
+      </c>
+      <c r="U39" s="5">
+        <f t="shared" si="53"/>
+        <v>0.39086294416243655</v>
+      </c>
+      <c r="V39" s="1">
+        <f t="shared" si="54"/>
+        <v>5.0897000000000006</v>
+      </c>
+      <c r="W39" s="3">
+        <f t="shared" si="55"/>
+        <v>3071.4621297370518</v>
+      </c>
+      <c r="X39" s="5">
+        <f t="shared" si="56"/>
+        <v>0.59417955452904725</v>
+      </c>
+      <c r="Y39" s="5">
+        <f t="shared" si="57"/>
+        <v>2.0138356164383562</v>
+      </c>
+      <c r="Z39">
+        <f t="shared" si="58"/>
+        <v>0.16111944910391102</v>
+      </c>
+      <c r="AA39">
+        <f t="shared" si="59"/>
+        <v>12.834939165904775</v>
+      </c>
+    </row>
+    <row r="40" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A40" s="8">
+        <v>39922</v>
+      </c>
+      <c r="C40">
+        <v>47</v>
+      </c>
+      <c r="D40" s="10">
+        <v>0.77</v>
+      </c>
+      <c r="E40" s="10">
+        <v>44</v>
+      </c>
+      <c r="F40" s="10">
+        <v>40</v>
+      </c>
+      <c r="G40">
+        <f t="shared" si="45"/>
+        <v>1760</v>
+      </c>
+      <c r="H40">
+        <v>15.25</v>
+      </c>
+      <c r="I40">
+        <v>1825</v>
+      </c>
+      <c r="J40" s="2">
+        <f t="shared" si="46"/>
+        <v>119.67213114754098</v>
+      </c>
+      <c r="K40" s="10">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="L40" s="3">
+        <v>4.37</v>
+      </c>
+      <c r="M40" s="10">
+        <v>37</v>
+      </c>
+      <c r="N40">
+        <f t="shared" si="47"/>
+        <v>299.2</v>
+      </c>
+      <c r="O40" s="1">
+        <f t="shared" si="48"/>
+        <v>6.0995989304812834</v>
+      </c>
+      <c r="P40">
+        <f t="shared" si="49"/>
+        <v>26840</v>
+      </c>
+      <c r="Q40" s="2">
+        <f t="shared" si="50"/>
+        <v>34857.142857142855</v>
+      </c>
+      <c r="R40" s="5">
+        <f t="shared" si="51"/>
+        <v>14.706849315068494</v>
+      </c>
+      <c r="S40" s="4">
+        <f t="shared" si="52"/>
+        <v>8.0585475699005444E-3</v>
+      </c>
+      <c r="T40" s="5">
+        <f t="shared" si="60"/>
+        <v>9.2697157914549216E-2</v>
+      </c>
+      <c r="U40" s="5">
+        <f t="shared" si="53"/>
+        <v>0.39086294416243655</v>
+      </c>
+      <c r="V40" s="1">
+        <f t="shared" si="54"/>
+        <v>5.0897000000000006</v>
+      </c>
+      <c r="W40" s="3">
+        <f t="shared" si="55"/>
+        <v>3071.4621297370518</v>
+      </c>
+      <c r="X40" s="5">
+        <f t="shared" si="56"/>
+        <v>0.59417955452904725</v>
+      </c>
+      <c r="Y40" s="5">
+        <f t="shared" si="57"/>
+        <v>2.5001643835616436</v>
+      </c>
+      <c r="Z40">
+        <f t="shared" si="58"/>
+        <v>0.12977870064853794</v>
+      </c>
+      <c r="AA40">
+        <f t="shared" si="59"/>
+        <v>10.516549880140145</v>
+      </c>
+    </row>
+    <row r="41" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A41" s="8">
+        <v>40122</v>
+      </c>
+      <c r="C41">
+        <v>49</v>
+      </c>
+      <c r="D41" s="10">
+        <v>0.9</v>
+      </c>
+      <c r="E41" s="10">
+        <v>42</v>
+      </c>
+      <c r="F41" s="10">
+        <v>40</v>
+      </c>
+      <c r="G41">
+        <f t="shared" si="45"/>
+        <v>1680</v>
+      </c>
+      <c r="H41">
+        <v>17.5</v>
+      </c>
+      <c r="I41">
+        <v>2425</v>
+      </c>
+      <c r="J41" s="2">
+        <f t="shared" si="46"/>
+        <v>138.57142857142858</v>
+      </c>
+      <c r="K41" s="10">
+        <v>0.8</v>
+      </c>
+      <c r="L41" s="3">
+        <v>4</v>
+      </c>
+      <c r="M41" s="10">
+        <v>18</v>
+      </c>
+      <c r="N41">
+        <f t="shared" si="47"/>
+        <v>258</v>
+      </c>
+      <c r="O41" s="1">
+        <f t="shared" si="48"/>
+        <v>9.3992248062015502</v>
+      </c>
+      <c r="P41">
+        <f t="shared" si="49"/>
+        <v>29400</v>
+      </c>
+      <c r="Q41" s="2">
+        <f t="shared" si="50"/>
+        <v>32666.666666666664</v>
+      </c>
+      <c r="R41" s="5">
+        <f t="shared" si="51"/>
+        <v>12.123711340206185</v>
+      </c>
+      <c r="S41" s="4">
+        <f t="shared" si="52"/>
+        <v>4.9994685938994574E-3</v>
+      </c>
+      <c r="T41" s="5">
+        <f t="shared" si="60"/>
+        <v>8.4541062801932368E-2</v>
+      </c>
+      <c r="U41" s="5">
+        <f t="shared" si="53"/>
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="V41" s="1">
+        <f t="shared" si="54"/>
+        <v>5.9490000000000007</v>
+      </c>
+      <c r="W41" s="3">
+        <f t="shared" si="55"/>
+        <v>3492.3807066414633</v>
+      </c>
+      <c r="X41" s="5">
+        <f t="shared" si="56"/>
+        <v>0.69436874261399262</v>
+      </c>
+      <c r="Y41" s="5">
+        <f t="shared" si="57"/>
+        <v>1.8618556701030926</v>
+      </c>
+      <c r="Z41">
+        <f t="shared" si="58"/>
+        <v>0.19182091441227653</v>
+      </c>
+      <c r="AA41">
+        <f t="shared" si="59"/>
+        <v>11.749031007751936</v>
+      </c>
+    </row>
+    <row r="42" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A42" s="8">
+        <v>38249</v>
+      </c>
+      <c r="C42">
+        <v>45</v>
+      </c>
+      <c r="D42" s="10">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="E42" s="10">
+        <v>33</v>
+      </c>
+      <c r="F42" s="10">
+        <v>40</v>
+      </c>
+      <c r="G42">
+        <f t="shared" si="45"/>
+        <v>1320</v>
+      </c>
+      <c r="H42">
+        <v>14</v>
+      </c>
+      <c r="I42">
+        <v>2425</v>
+      </c>
+      <c r="J42" s="2">
+        <f t="shared" si="46"/>
+        <v>173.21428571428572</v>
+      </c>
+      <c r="K42" s="10">
+        <v>0.75</v>
+      </c>
+      <c r="L42" s="3">
+        <v>4</v>
+      </c>
+      <c r="M42" s="10">
+        <v>36</v>
+      </c>
+      <c r="N42">
+        <f t="shared" si="47"/>
+        <v>276</v>
+      </c>
+      <c r="O42" s="1">
+        <f t="shared" si="48"/>
+        <v>8.7862318840579707</v>
+      </c>
+      <c r="P42">
+        <f t="shared" si="49"/>
+        <v>18480</v>
+      </c>
+      <c r="Q42" s="2">
+        <f t="shared" si="50"/>
+        <v>33600</v>
+      </c>
+      <c r="R42" s="5">
+        <f t="shared" si="51"/>
+        <v>7.6206185567010305</v>
+      </c>
+      <c r="S42" s="4">
+        <f t="shared" si="52"/>
+        <v>3.1425231161653733E-3</v>
+      </c>
+      <c r="T42" s="5">
+        <f t="shared" si="60"/>
+        <v>0.1152832674571805</v>
+      </c>
+      <c r="U42" s="5">
+        <f t="shared" si="53"/>
+        <v>0.31428571428571433</v>
+      </c>
+      <c r="V42" s="1">
+        <f t="shared" si="54"/>
+        <v>3.6355000000000004</v>
+      </c>
+      <c r="W42" s="3">
+        <f t="shared" si="55"/>
+        <v>3196.6601771382916</v>
+      </c>
+      <c r="X42" s="5">
+        <f t="shared" si="56"/>
+        <v>0.75860425119410224</v>
+      </c>
+      <c r="Y42" s="5">
+        <f t="shared" si="57"/>
+        <v>1.5934020618556701</v>
+      </c>
+      <c r="Z42">
+        <f t="shared" si="58"/>
+        <v>0.19524959742351047</v>
+      </c>
+      <c r="AA42">
+        <f t="shared" si="59"/>
+        <v>11.714975845410628</v>
+      </c>
+    </row>
+    <row r="43" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A43" s="8">
+        <v>38375</v>
+      </c>
+      <c r="C43">
+        <v>45</v>
+      </c>
+      <c r="D43" s="10">
+        <v>0.61</v>
+      </c>
+      <c r="E43" s="10">
+        <v>35</v>
+      </c>
+      <c r="F43" s="10">
+        <v>40</v>
+      </c>
+      <c r="G43">
+        <f t="shared" si="45"/>
+        <v>1400</v>
+      </c>
+      <c r="H43">
+        <v>14.5</v>
+      </c>
+      <c r="I43">
+        <v>1775</v>
+      </c>
+      <c r="J43" s="2">
+        <f t="shared" si="46"/>
+        <v>122.41379310344827</v>
+      </c>
+      <c r="K43" s="10">
+        <v>0.4</v>
+      </c>
+      <c r="L43" s="3">
+        <v>4</v>
+      </c>
+      <c r="M43" s="10">
+        <v>29</v>
+      </c>
+      <c r="N43">
+        <f t="shared" ref="N43:N60" si="61">L43*60+M43</f>
+        <v>269</v>
+      </c>
+      <c r="O43" s="1">
+        <f t="shared" ref="O43:O60" si="62">I43/N43</f>
+        <v>6.5985130111524164</v>
+      </c>
+      <c r="P43">
+        <f t="shared" si="49"/>
+        <v>20300</v>
+      </c>
+      <c r="Q43" s="2">
+        <f t="shared" si="50"/>
+        <v>33278.688524590165</v>
+      </c>
+      <c r="R43" s="5">
+        <f t="shared" si="51"/>
+        <v>11.43661971830986</v>
+      </c>
+      <c r="S43" s="4">
+        <f t="shared" si="52"/>
+        <v>6.4431660384844285E-3</v>
+      </c>
+      <c r="T43" s="5">
+        <f t="shared" si="60"/>
+        <v>0.10750772154906153</v>
+      </c>
+      <c r="U43" s="5">
+        <f t="shared" si="53"/>
+        <v>0.33701657458563533</v>
+      </c>
+      <c r="V43" s="1">
+        <f t="shared" si="54"/>
+        <v>4.0320999999999998</v>
+      </c>
+      <c r="W43" s="3">
+        <f t="shared" si="55"/>
+        <v>3199.4317322992915</v>
+      </c>
+      <c r="X43" s="5">
+        <f t="shared" si="56"/>
+        <v>0.55478602093015594</v>
+      </c>
+      <c r="Y43" s="5">
+        <f t="shared" ref="Y43:Y60" si="63">N43/J43</f>
+        <v>2.1974647887323946</v>
+      </c>
+      <c r="Z43">
+        <f t="shared" ref="Z43:Z60" si="64">O43/C43</f>
+        <v>0.14663362247005371</v>
+      </c>
+      <c r="AA43">
+        <f t="shared" ref="AA43:AA60" si="65">O43/K43</f>
+        <v>16.496282527881039</v>
+      </c>
+    </row>
+    <row r="44" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A44" s="8">
+        <v>38375</v>
+      </c>
+      <c r="C44">
+        <v>45</v>
+      </c>
+      <c r="D44" s="10">
+        <v>0.61</v>
+      </c>
+      <c r="E44" s="10">
+        <v>35</v>
+      </c>
+      <c r="F44" s="10">
+        <v>40</v>
+      </c>
+      <c r="G44">
+        <f t="shared" si="45"/>
+        <v>1400</v>
+      </c>
+      <c r="H44">
+        <v>14.5</v>
+      </c>
+      <c r="I44">
+        <v>1800</v>
+      </c>
+      <c r="J44" s="2">
+        <f t="shared" si="46"/>
+        <v>124.13793103448276</v>
+      </c>
+      <c r="K44" s="10">
+        <v>0.4</v>
+      </c>
+      <c r="L44" s="3">
+        <v>4</v>
+      </c>
+      <c r="M44" s="10">
+        <v>40</v>
+      </c>
+      <c r="N44">
+        <f t="shared" si="61"/>
+        <v>280</v>
+      </c>
+      <c r="O44" s="1">
+        <f t="shared" si="62"/>
+        <v>6.4285714285714288</v>
+      </c>
+      <c r="P44">
+        <f t="shared" si="49"/>
+        <v>20300</v>
+      </c>
+      <c r="Q44" s="2">
+        <f t="shared" si="50"/>
+        <v>33278.688524590165</v>
+      </c>
+      <c r="R44" s="5">
+        <f t="shared" si="51"/>
+        <v>11.277777777777779</v>
+      </c>
+      <c r="S44" s="4">
+        <f t="shared" si="52"/>
+        <v>6.2654320987654329E-3</v>
+      </c>
+      <c r="T44" s="5">
+        <f t="shared" si="60"/>
+        <v>0.10750772154906153</v>
+      </c>
+      <c r="U44" s="5">
+        <f t="shared" si="53"/>
+        <v>0.33701657458563533</v>
+      </c>
+      <c r="V44" s="1">
+        <f t="shared" si="54"/>
+        <v>4.0320999999999998</v>
+      </c>
+      <c r="W44" s="3">
+        <f t="shared" si="55"/>
+        <v>3199.4317322992915</v>
+      </c>
+      <c r="X44" s="5">
+        <f t="shared" si="56"/>
+        <v>0.56259990854889064</v>
+      </c>
+      <c r="Y44" s="5">
+        <f t="shared" si="63"/>
+        <v>2.2555555555555555</v>
+      </c>
+      <c r="Z44">
+        <f t="shared" si="64"/>
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="AA44">
+        <f t="shared" si="65"/>
+        <v>16.071428571428569</v>
+      </c>
+    </row>
+    <row r="45" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A45" s="8">
+        <v>38431</v>
+      </c>
+      <c r="C45">
+        <v>45</v>
+      </c>
+      <c r="D45" s="10">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="E45" s="10">
+        <v>33</v>
+      </c>
+      <c r="F45" s="10">
+        <v>40</v>
+      </c>
+      <c r="G45">
+        <f t="shared" si="45"/>
+        <v>1320</v>
+      </c>
+      <c r="H45">
+        <v>14</v>
+      </c>
+      <c r="I45">
+        <v>1885</v>
+      </c>
+      <c r="J45" s="2">
+        <f t="shared" si="46"/>
+        <v>134.64285714285714</v>
+      </c>
+      <c r="K45" s="10">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="L45" s="3">
+        <v>4</v>
+      </c>
+      <c r="M45" s="10">
+        <v>16</v>
+      </c>
+      <c r="N45">
+        <f t="shared" si="61"/>
+        <v>256</v>
+      </c>
+      <c r="O45" s="1">
+        <f t="shared" si="62"/>
+        <v>7.36328125</v>
+      </c>
+      <c r="P45">
+        <f t="shared" si="49"/>
+        <v>18480</v>
+      </c>
+      <c r="Q45" s="2">
+        <f t="shared" si="50"/>
+        <v>31862.068965517243</v>
+      </c>
+      <c r="R45" s="5">
+        <f t="shared" si="51"/>
+        <v>9.8037135278514587</v>
+      </c>
+      <c r="S45" s="4">
+        <f t="shared" si="52"/>
+        <v>5.2009090333429491E-3</v>
+      </c>
+      <c r="T45" s="5">
+        <f t="shared" si="60"/>
+        <v>0.1111944027986007</v>
+      </c>
+      <c r="U45" s="5">
+        <f t="shared" si="53"/>
+        <v>0.3258426966292135</v>
+      </c>
+      <c r="V45" s="1">
+        <f t="shared" si="54"/>
+        <v>3.8338000000000001</v>
+      </c>
+      <c r="W45" s="3">
+        <f t="shared" si="55"/>
+        <v>3112.8903185414301</v>
+      </c>
+      <c r="X45" s="5">
+        <f t="shared" si="56"/>
+        <v>0.60554655227403964</v>
+      </c>
+      <c r="Y45" s="5">
+        <f t="shared" si="63"/>
+        <v>1.9013262599469496</v>
+      </c>
+      <c r="Z45">
+        <f t="shared" si="64"/>
+        <v>0.16362847222222221</v>
+      </c>
+      <c r="AA45">
+        <f t="shared" si="65"/>
+        <v>13.38778409090909</v>
+      </c>
+    </row>
+    <row r="46" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A46" s="8">
+        <v>38445</v>
+      </c>
+      <c r="C46">
+        <v>45</v>
+      </c>
+      <c r="D46" s="10">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="E46" s="10">
+        <v>33</v>
+      </c>
+      <c r="F46" s="10">
+        <v>40</v>
+      </c>
+      <c r="G46">
+        <f t="shared" si="45"/>
+        <v>1320</v>
+      </c>
+      <c r="H46">
+        <v>14</v>
+      </c>
+      <c r="I46">
+        <v>1775</v>
+      </c>
+      <c r="J46" s="2">
+        <f t="shared" si="46"/>
+        <v>126.78571428571429</v>
+      </c>
+      <c r="K46" s="10">
+        <v>0.4</v>
+      </c>
+      <c r="L46" s="3">
+        <v>4</v>
+      </c>
+      <c r="M46" s="10">
+        <v>30</v>
+      </c>
+      <c r="N46">
+        <f t="shared" si="61"/>
+        <v>270</v>
+      </c>
+      <c r="O46" s="1">
+        <f t="shared" si="62"/>
+        <v>6.5740740740740744</v>
+      </c>
+      <c r="P46">
+        <f t="shared" si="49"/>
+        <v>18480</v>
+      </c>
+      <c r="Q46" s="2">
+        <f t="shared" si="50"/>
+        <v>32421.05263157895</v>
+      </c>
+      <c r="R46" s="5">
+        <f t="shared" si="51"/>
+        <v>10.411267605633803</v>
+      </c>
+      <c r="S46" s="4">
+        <f t="shared" si="52"/>
+        <v>5.8655028764134105E-3</v>
+      </c>
+      <c r="T46" s="5">
+        <f t="shared" si="60"/>
+        <v>0.11250953470633104</v>
+      </c>
+      <c r="U46" s="5">
+        <f t="shared" si="53"/>
+        <v>0.32203389830508472</v>
+      </c>
+      <c r="V46" s="1">
+        <f t="shared" si="54"/>
+        <v>3.7677</v>
+      </c>
+      <c r="W46" s="3">
+        <f t="shared" si="55"/>
+        <v>3140.0776497427632</v>
+      </c>
+      <c r="X46" s="5">
+        <f t="shared" si="56"/>
+        <v>0.56527264545365907</v>
+      </c>
+      <c r="Y46" s="5">
+        <f t="shared" si="63"/>
+        <v>2.1295774647887322</v>
+      </c>
+      <c r="Z46">
+        <f t="shared" si="64"/>
+        <v>0.14609053497942387</v>
+      </c>
+      <c r="AA46">
+        <f t="shared" si="65"/>
+        <v>16.435185185185183</v>
+      </c>
+    </row>
+    <row r="47" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A47" s="8">
+        <v>38445</v>
+      </c>
+      <c r="C47">
+        <v>45</v>
+      </c>
+      <c r="D47" s="10">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="E47" s="10">
+        <v>33</v>
+      </c>
+      <c r="F47" s="10">
+        <v>40</v>
+      </c>
+      <c r="G47">
+        <f t="shared" si="45"/>
+        <v>1320</v>
+      </c>
+      <c r="H47">
+        <v>14</v>
+      </c>
+      <c r="I47">
+        <v>1858</v>
+      </c>
+      <c r="J47" s="2">
+        <f t="shared" si="46"/>
+        <v>132.71428571428572</v>
+      </c>
+      <c r="L47" s="3">
+        <v>4</v>
+      </c>
+      <c r="M47" s="10">
+        <v>32</v>
+      </c>
+      <c r="N47">
+        <f t="shared" si="61"/>
+        <v>272</v>
+      </c>
+      <c r="O47" s="1">
+        <f t="shared" si="62"/>
+        <v>6.8308823529411766</v>
+      </c>
+      <c r="P47">
+        <f t="shared" si="49"/>
+        <v>18480</v>
+      </c>
+      <c r="Q47" s="2">
+        <f t="shared" si="50"/>
+        <v>32421.05263157895</v>
+      </c>
+      <c r="R47" s="5">
+        <f t="shared" si="51"/>
+        <v>9.9461786867599571</v>
+      </c>
+      <c r="S47" s="4">
+        <f t="shared" si="52"/>
+        <v>5.3531639864154773E-3</v>
+      </c>
+      <c r="T47" s="5">
+        <f t="shared" si="60"/>
+        <v>0.11250953470633104</v>
+      </c>
+      <c r="U47" s="5">
+        <f t="shared" si="53"/>
+        <v>0.32203389830508472</v>
+      </c>
+      <c r="V47" s="1">
+        <f t="shared" si="54"/>
+        <v>3.7677</v>
+      </c>
+      <c r="W47" s="3">
+        <f t="shared" si="55"/>
+        <v>3140.0776497427632</v>
+      </c>
+      <c r="X47" s="5">
+        <f t="shared" si="56"/>
+        <v>0.59170511281853433</v>
+      </c>
+      <c r="Y47" s="5">
+        <f t="shared" si="63"/>
+        <v>2.0495156081808394</v>
+      </c>
+      <c r="Z47">
+        <f t="shared" si="64"/>
+        <v>0.15179738562091505</v>
+      </c>
+    </row>
+    <row r="48" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A48" s="8">
+        <v>40559</v>
+      </c>
+      <c r="C48">
+        <v>45</v>
+      </c>
+      <c r="D48" s="10">
+        <v>0.8</v>
+      </c>
+      <c r="E48" s="10">
+        <v>39</v>
+      </c>
+      <c r="F48" s="10">
+        <v>40</v>
+      </c>
+      <c r="G48">
+        <f t="shared" si="45"/>
+        <v>1560</v>
+      </c>
+      <c r="H48">
+        <v>17.5</v>
+      </c>
+      <c r="I48">
+        <v>1750</v>
+      </c>
+      <c r="J48" s="2">
+        <f t="shared" si="46"/>
+        <v>100</v>
+      </c>
+      <c r="K48">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="L48" s="3">
+        <v>4</v>
+      </c>
+      <c r="M48" s="10">
+        <v>18</v>
+      </c>
+      <c r="N48">
+        <f t="shared" si="61"/>
+        <v>258</v>
+      </c>
+      <c r="O48" s="1">
+        <f t="shared" si="62"/>
+        <v>6.7829457364341081</v>
+      </c>
+      <c r="P48">
+        <f t="shared" si="49"/>
+        <v>27300</v>
+      </c>
+      <c r="Q48" s="2">
+        <f t="shared" si="50"/>
+        <v>34125</v>
+      </c>
+      <c r="R48" s="5">
+        <f t="shared" si="51"/>
+        <v>15.6</v>
+      </c>
+      <c r="S48" s="4">
+        <f t="shared" si="52"/>
+        <v>8.9142857142857149E-3</v>
+      </c>
+      <c r="T48" s="5">
+        <f t="shared" si="60"/>
+        <v>9.0579710144927522E-2</v>
+      </c>
+      <c r="U48" s="5">
+        <f t="shared" si="53"/>
+        <v>0.4</v>
+      </c>
+      <c r="V48" s="1">
+        <f t="shared" si="54"/>
+        <v>5.2880000000000003</v>
+      </c>
+      <c r="W48" s="3">
+        <f t="shared" si="55"/>
+        <v>3704.229120226868</v>
+      </c>
+      <c r="X48" s="5">
+        <f t="shared" si="56"/>
+        <v>0.47243297949475116</v>
+      </c>
+      <c r="Y48" s="5">
+        <f t="shared" si="63"/>
+        <v>2.58</v>
+      </c>
+      <c r="Z48">
+        <f t="shared" si="64"/>
+        <v>0.15073212747631351</v>
+      </c>
+      <c r="AA48">
+        <f t="shared" si="65"/>
+        <v>12.332628611698377</v>
+      </c>
+    </row>
+    <row r="49" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A49" s="8">
+        <v>40594</v>
+      </c>
+      <c r="C49">
+        <v>45</v>
+      </c>
+      <c r="D49" s="10">
+        <v>0.84</v>
+      </c>
+      <c r="E49" s="10">
+        <v>39</v>
+      </c>
+      <c r="F49" s="10">
+        <v>40</v>
+      </c>
+      <c r="G49">
+        <f t="shared" si="45"/>
+        <v>1560</v>
+      </c>
+      <c r="H49">
+        <v>17.5</v>
+      </c>
+      <c r="I49">
+        <v>2400</v>
+      </c>
+      <c r="J49" s="2">
+        <f t="shared" si="46"/>
+        <v>137.14285714285714</v>
+      </c>
+      <c r="K49">
+        <v>0.6</v>
+      </c>
+      <c r="L49" s="3">
+        <v>4</v>
+      </c>
+      <c r="M49" s="10">
+        <v>8</v>
+      </c>
+      <c r="N49">
+        <f t="shared" si="61"/>
+        <v>248</v>
+      </c>
+      <c r="O49" s="1">
+        <f t="shared" si="62"/>
+        <v>9.67741935483871</v>
+      </c>
+      <c r="P49">
+        <f t="shared" si="49"/>
+        <v>27300</v>
+      </c>
+      <c r="Q49" s="2">
+        <f t="shared" si="50"/>
+        <v>32500</v>
+      </c>
+      <c r="R49" s="5">
+        <f t="shared" si="51"/>
+        <v>11.375</v>
+      </c>
+      <c r="S49" s="4">
+        <f t="shared" si="52"/>
+        <v>4.7395833333333335E-3</v>
+      </c>
+      <c r="T49" s="5">
+        <f t="shared" si="60"/>
+        <v>8.7991718426501039E-2</v>
+      </c>
+      <c r="U49" s="5">
+        <f t="shared" si="53"/>
+        <v>0.41176470588235292</v>
+      </c>
+      <c r="V49" s="1">
+        <f t="shared" si="54"/>
+        <v>5.5524000000000004</v>
+      </c>
+      <c r="W49" s="3">
+        <f t="shared" si="55"/>
+        <v>3614.9574686474812</v>
+      </c>
+      <c r="X49" s="5">
+        <f t="shared" si="56"/>
+        <v>0.66390822597919763</v>
+      </c>
+      <c r="Y49" s="5">
+        <f t="shared" si="63"/>
+        <v>1.8083333333333333</v>
+      </c>
+      <c r="Z49">
+        <f t="shared" si="64"/>
+        <v>0.21505376344086022</v>
+      </c>
+      <c r="AA49">
+        <f t="shared" si="65"/>
+        <v>16.129032258064516</v>
+      </c>
+    </row>
+    <row r="50" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A50" s="8">
+        <v>40895</v>
+      </c>
+      <c r="C50">
+        <v>45</v>
+      </c>
+      <c r="D50" s="10">
+        <v>0.9</v>
+      </c>
+      <c r="E50" s="10">
+        <v>39</v>
+      </c>
+      <c r="F50" s="10">
+        <v>40</v>
+      </c>
+      <c r="G50">
+        <f t="shared" si="45"/>
+        <v>1560</v>
+      </c>
+      <c r="H50">
+        <v>17</v>
+      </c>
+      <c r="I50">
+        <v>2200</v>
+      </c>
+      <c r="J50" s="2">
+        <f t="shared" si="46"/>
+        <v>129.41176470588235</v>
+      </c>
+      <c r="K50">
+        <v>-0.75</v>
+      </c>
+      <c r="L50" s="3">
+        <v>4</v>
+      </c>
+      <c r="M50" s="10">
+        <v>29</v>
+      </c>
+      <c r="N50">
+        <f t="shared" si="61"/>
+        <v>269</v>
+      </c>
+      <c r="O50" s="1">
+        <f t="shared" si="62"/>
+        <v>8.1784386617100377</v>
+      </c>
+      <c r="P50">
+        <f t="shared" si="49"/>
+        <v>26520</v>
+      </c>
+      <c r="Q50" s="2">
+        <f t="shared" si="50"/>
+        <v>29466.666666666664</v>
+      </c>
+      <c r="R50" s="5">
+        <f t="shared" si="51"/>
+        <v>12.054545454545455</v>
+      </c>
+      <c r="S50" s="4">
+        <f t="shared" si="52"/>
+        <v>5.4793388429752064E-3</v>
+      </c>
+      <c r="T50" s="5">
+        <f t="shared" si="60"/>
+        <v>8.4541062801932368E-2</v>
+      </c>
+      <c r="U50" s="5">
+        <f t="shared" si="53"/>
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="V50" s="1">
+        <f t="shared" si="54"/>
+        <v>5.9490000000000007</v>
+      </c>
+      <c r="W50" s="3">
+        <f t="shared" si="55"/>
+        <v>3343.7814901922375</v>
+      </c>
+      <c r="X50" s="5">
+        <f t="shared" si="56"/>
+        <v>0.65793772902113878</v>
+      </c>
+      <c r="Y50" s="5">
+        <f t="shared" si="63"/>
+        <v>2.0786363636363636</v>
+      </c>
+      <c r="Z50">
+        <f t="shared" si="64"/>
+        <v>0.18174308137133416</v>
+      </c>
+      <c r="AA50">
+        <f t="shared" si="65"/>
+        <v>-10.90458488228005</v>
+      </c>
+    </row>
+    <row r="51" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A51" s="8">
+        <v>40895</v>
+      </c>
+      <c r="C51">
+        <v>45</v>
+      </c>
+      <c r="D51" s="10">
+        <v>0.9</v>
+      </c>
+      <c r="E51" s="10">
+        <v>39</v>
+      </c>
+      <c r="F51" s="10">
+        <v>40</v>
+      </c>
+      <c r="G51">
+        <f t="shared" si="45"/>
+        <v>1560</v>
+      </c>
+      <c r="H51">
+        <v>17</v>
+      </c>
+      <c r="I51">
+        <v>2175</v>
+      </c>
+      <c r="J51" s="2">
+        <f t="shared" si="46"/>
+        <v>127.94117647058823</v>
+      </c>
+      <c r="K51">
+        <v>0.7</v>
+      </c>
+      <c r="L51" s="3">
+        <v>4</v>
+      </c>
+      <c r="M51" s="10">
+        <v>5</v>
+      </c>
+      <c r="N51">
+        <f t="shared" si="61"/>
+        <v>245</v>
+      </c>
+      <c r="O51" s="1">
+        <f t="shared" si="62"/>
+        <v>8.8775510204081627</v>
+      </c>
+      <c r="P51">
+        <f t="shared" si="49"/>
+        <v>26520</v>
+      </c>
+      <c r="Q51" s="2">
+        <f t="shared" si="50"/>
+        <v>29466.666666666664</v>
+      </c>
+      <c r="R51" s="5">
+        <f t="shared" si="51"/>
+        <v>12.193103448275862</v>
+      </c>
+      <c r="S51" s="4">
+        <f t="shared" si="52"/>
+        <v>5.6060245739199361E-3</v>
+      </c>
+      <c r="T51" s="5">
+        <f t="shared" si="60"/>
+        <v>8.4541062801932368E-2</v>
+      </c>
+      <c r="U51" s="5">
+        <f t="shared" si="53"/>
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="V51" s="1">
+        <f t="shared" si="54"/>
+        <v>5.9490000000000007</v>
+      </c>
+      <c r="W51" s="3">
+        <f t="shared" si="55"/>
+        <v>3343.7814901922375</v>
+      </c>
+      <c r="X51" s="5">
+        <f t="shared" si="56"/>
+        <v>0.65046116391862585</v>
+      </c>
+      <c r="Y51" s="5">
+        <f t="shared" si="63"/>
+        <v>1.9149425287356323</v>
+      </c>
+      <c r="Z51">
+        <f t="shared" si="64"/>
+        <v>0.19727891156462585</v>
+      </c>
+      <c r="AA51">
+        <f t="shared" si="65"/>
+        <v>12.682215743440233</v>
+      </c>
+    </row>
+    <row r="52" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A52" s="8">
+        <v>38445</v>
+      </c>
+      <c r="C52">
+        <v>45</v>
+      </c>
+      <c r="D52" s="10">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="E52" s="10">
+        <v>35</v>
+      </c>
+      <c r="F52" s="10">
+        <v>40</v>
+      </c>
+      <c r="G52">
+        <f t="shared" si="45"/>
+        <v>1400</v>
+      </c>
+      <c r="H52">
+        <v>14</v>
+      </c>
+      <c r="I52">
+        <v>1800</v>
+      </c>
+      <c r="J52" s="2">
+        <f t="shared" si="46"/>
+        <v>128.57142857142858</v>
+      </c>
+      <c r="K52">
+        <v>0.45</v>
+      </c>
+      <c r="L52" s="3">
+        <v>4</v>
+      </c>
+      <c r="M52" s="10">
+        <v>25</v>
+      </c>
+      <c r="N52">
+        <f t="shared" si="61"/>
+        <v>265</v>
+      </c>
+      <c r="O52" s="1">
+        <f t="shared" si="62"/>
+        <v>6.7924528301886795</v>
+      </c>
+      <c r="P52">
+        <f t="shared" si="49"/>
+        <v>19600</v>
+      </c>
+      <c r="Q52" s="2">
+        <f t="shared" si="50"/>
+        <v>34385.964912280702</v>
+      </c>
+      <c r="R52" s="5">
+        <f t="shared" si="51"/>
+        <v>10.888888888888889</v>
+      </c>
+      <c r="S52" s="4">
+        <f t="shared" si="52"/>
+        <v>6.0493827160493828E-3</v>
+      </c>
+      <c r="T52" s="5">
+        <f t="shared" si="60"/>
+        <v>0.11250953470633104</v>
+      </c>
+      <c r="U52" s="5">
+        <f t="shared" si="53"/>
+        <v>0.32203389830508472</v>
+      </c>
+      <c r="V52" s="1">
+        <f t="shared" si="54"/>
+        <v>3.7677</v>
+      </c>
+      <c r="W52" s="3">
+        <f t="shared" si="55"/>
+        <v>3140.0776497427632</v>
+      </c>
+      <c r="X52" s="5">
+        <f t="shared" si="56"/>
+        <v>0.57323423200934442</v>
+      </c>
+      <c r="Y52" s="5">
+        <f t="shared" si="63"/>
+        <v>2.0611111111111109</v>
+      </c>
+      <c r="Z52">
+        <f t="shared" si="64"/>
+        <v>0.15094339622641509</v>
+      </c>
+      <c r="AA52">
+        <f t="shared" si="65"/>
+        <v>15.09433962264151</v>
+      </c>
+    </row>
+    <row r="53" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A53" s="8">
+        <v>40923</v>
+      </c>
+      <c r="C53">
+        <v>45</v>
+      </c>
+      <c r="D53" s="10">
+        <v>0.75</v>
+      </c>
+      <c r="E53" s="10">
+        <v>44</v>
+      </c>
+      <c r="F53" s="10">
+        <v>40</v>
+      </c>
+      <c r="G53">
+        <f t="shared" si="45"/>
+        <v>1760</v>
+      </c>
+      <c r="H53">
+        <v>15</v>
+      </c>
+      <c r="I53">
+        <v>1700</v>
+      </c>
+      <c r="J53" s="2">
+        <f t="shared" si="46"/>
+        <v>113.33333333333333</v>
+      </c>
+      <c r="K53">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="L53" s="3">
+        <v>4</v>
+      </c>
+      <c r="M53" s="10">
+        <v>32</v>
+      </c>
+      <c r="N53">
+        <f t="shared" si="61"/>
+        <v>272</v>
+      </c>
+      <c r="O53" s="1">
+        <f t="shared" si="62"/>
+        <v>6.25</v>
+      </c>
+      <c r="P53">
+        <f t="shared" si="49"/>
+        <v>26400</v>
+      </c>
+      <c r="Q53" s="2">
+        <f t="shared" si="50"/>
+        <v>35200</v>
+      </c>
+      <c r="R53" s="5">
+        <f t="shared" si="51"/>
+        <v>15.529411764705882</v>
+      </c>
+      <c r="S53" s="4">
+        <f t="shared" si="52"/>
+        <v>9.1349480968858122E-3</v>
+      </c>
+      <c r="T53" s="5">
+        <f t="shared" si="60"/>
+        <v>9.420289855072464E-2</v>
+      </c>
+      <c r="U53" s="5">
+        <f t="shared" si="53"/>
+        <v>0.38461538461538464</v>
+      </c>
+      <c r="V53" s="1">
+        <f t="shared" si="54"/>
+        <v>4.9575000000000005</v>
+      </c>
+      <c r="W53" s="3">
+        <f t="shared" si="55"/>
+        <v>3035.9318537312397</v>
+      </c>
+      <c r="X53" s="5">
+        <f t="shared" si="56"/>
+        <v>0.55995986797617192</v>
+      </c>
+      <c r="Y53" s="5">
+        <f t="shared" si="63"/>
+        <v>2.4</v>
+      </c>
+      <c r="Z53">
+        <f t="shared" si="64"/>
+        <v>0.1388888888888889</v>
+      </c>
+      <c r="AA53">
+        <f t="shared" si="65"/>
+        <v>11.363636363636363</v>
+      </c>
+    </row>
+    <row r="54" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A54" s="8">
+        <v>40923</v>
+      </c>
+      <c r="C54">
+        <v>45</v>
+      </c>
+      <c r="D54" s="10">
+        <v>0.75</v>
+      </c>
+      <c r="E54" s="10">
+        <v>44</v>
+      </c>
+      <c r="F54" s="10">
+        <v>40</v>
+      </c>
+      <c r="G54">
+        <f t="shared" si="45"/>
+        <v>1760</v>
+      </c>
+      <c r="H54">
+        <v>15</v>
+      </c>
+      <c r="I54">
+        <v>1600</v>
+      </c>
+      <c r="J54" s="2">
+        <f t="shared" si="46"/>
+        <v>106.66666666666667</v>
+      </c>
+      <c r="K54">
+        <v>0.45</v>
+      </c>
+      <c r="L54" s="3">
+        <v>4</v>
+      </c>
+      <c r="M54" s="10">
+        <v>21</v>
+      </c>
+      <c r="N54">
+        <f t="shared" si="61"/>
+        <v>261</v>
+      </c>
+      <c r="O54" s="1">
+        <f t="shared" si="62"/>
+        <v>6.1302681992337167</v>
+      </c>
+      <c r="P54">
+        <f t="shared" si="49"/>
+        <v>26400</v>
+      </c>
+      <c r="Q54" s="2">
+        <f t="shared" si="50"/>
+        <v>35200</v>
+      </c>
+      <c r="R54" s="5">
+        <f t="shared" si="51"/>
+        <v>16.5</v>
+      </c>
+      <c r="S54" s="4">
+        <f t="shared" si="52"/>
+        <v>1.03125E-2</v>
+      </c>
+      <c r="T54" s="5">
+        <f t="shared" si="60"/>
+        <v>9.420289855072464E-2</v>
+      </c>
+      <c r="U54" s="5">
+        <f t="shared" si="53"/>
+        <v>0.38461538461538464</v>
+      </c>
+      <c r="V54" s="1">
+        <f t="shared" si="54"/>
+        <v>4.9575000000000005</v>
+      </c>
+      <c r="W54" s="3">
+        <f t="shared" si="55"/>
+        <v>3035.9318537312397</v>
+      </c>
+      <c r="X54" s="5">
+        <f t="shared" si="56"/>
+        <v>0.52702105221286777</v>
+      </c>
+      <c r="Y54" s="5">
+        <f t="shared" si="63"/>
+        <v>2.4468749999999999</v>
+      </c>
+      <c r="Z54">
+        <f t="shared" si="64"/>
+        <v>0.1362281822051937</v>
+      </c>
+      <c r="AA54">
+        <f t="shared" si="65"/>
+        <v>13.62281822051937</v>
+      </c>
+    </row>
+    <row r="55" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A55" s="8">
+        <v>40923</v>
+      </c>
+      <c r="C55">
+        <v>45</v>
+      </c>
+      <c r="D55" s="10">
+        <v>0.75</v>
+      </c>
+      <c r="E55" s="10">
+        <v>44</v>
+      </c>
+      <c r="F55" s="10">
+        <v>40</v>
+      </c>
+      <c r="G55">
+        <f t="shared" si="45"/>
+        <v>1760</v>
+      </c>
+      <c r="H55">
+        <v>15</v>
+      </c>
+      <c r="I55">
+        <v>1650</v>
+      </c>
+      <c r="J55" s="2">
+        <f t="shared" si="46"/>
+        <v>110</v>
+      </c>
+      <c r="K55">
+        <v>0.5</v>
+      </c>
+      <c r="L55" s="3">
+        <v>4</v>
+      </c>
+      <c r="M55" s="10">
+        <v>2</v>
+      </c>
+      <c r="N55">
+        <f t="shared" si="61"/>
+        <v>242</v>
+      </c>
+      <c r="O55" s="1">
+        <f t="shared" si="62"/>
+        <v>6.8181818181818183</v>
+      </c>
+      <c r="P55">
+        <f t="shared" si="49"/>
+        <v>26400</v>
+      </c>
+      <c r="Q55" s="2">
+        <f t="shared" si="50"/>
+        <v>35200</v>
+      </c>
+      <c r="R55" s="5">
+        <f t="shared" si="51"/>
+        <v>16</v>
+      </c>
+      <c r="S55" s="4">
+        <f t="shared" si="52"/>
+        <v>9.696969696969697E-3</v>
+      </c>
+      <c r="T55" s="5">
+        <f t="shared" si="60"/>
+        <v>9.420289855072464E-2</v>
+      </c>
+      <c r="U55" s="5">
+        <f t="shared" si="53"/>
+        <v>0.38461538461538464</v>
+      </c>
+      <c r="V55" s="1">
+        <f t="shared" si="54"/>
+        <v>4.9575000000000005</v>
+      </c>
+      <c r="W55" s="3">
+        <f t="shared" si="55"/>
+        <v>3035.9318537312397</v>
+      </c>
+      <c r="X55" s="5">
+        <f t="shared" si="56"/>
+        <v>0.54349046009451984</v>
+      </c>
+      <c r="Y55" s="5">
+        <f t="shared" si="63"/>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="Z55">
+        <f t="shared" si="64"/>
+        <v>0.15151515151515152</v>
+      </c>
+      <c r="AA55">
+        <f t="shared" si="65"/>
+        <v>13.636363636363637</v>
+      </c>
+    </row>
+    <row r="56" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A56" s="8">
+        <v>40923</v>
+      </c>
+      <c r="C56">
+        <v>45</v>
+      </c>
+      <c r="D56" s="10">
+        <v>0.99</v>
+      </c>
+      <c r="H56">
+        <v>19</v>
+      </c>
+      <c r="I56">
+        <v>2300</v>
+      </c>
+      <c r="J56" s="2">
+        <f t="shared" si="46"/>
+        <v>121.05263157894737</v>
+      </c>
+      <c r="K56">
+        <v>0.5</v>
+      </c>
+      <c r="L56" s="3">
+        <v>4</v>
+      </c>
+      <c r="M56" s="10">
+        <v>16</v>
+      </c>
+      <c r="N56">
+        <f t="shared" si="61"/>
+        <v>256</v>
+      </c>
+      <c r="O56" s="1">
+        <f t="shared" si="62"/>
+        <v>8.984375</v>
+      </c>
+      <c r="P56">
+        <f t="shared" ref="P56:P60" si="66">G56*H56</f>
+        <v>0</v>
+      </c>
+      <c r="Q56" s="2">
+        <f t="shared" ref="Q56:Q60" si="67">P56/D56</f>
+        <v>0</v>
+      </c>
+      <c r="R56" s="5">
+        <f t="shared" ref="R56:R60" si="68">P56/I56</f>
+        <v>0</v>
+      </c>
+      <c r="S56" s="4">
+        <f t="shared" ref="S56:S60" si="69">R56/I56</f>
+        <v>0</v>
+      </c>
+      <c r="T56" s="5">
+        <f t="shared" si="60"/>
+        <v>8.014931927975405E-2</v>
+      </c>
+      <c r="U56" s="5">
+        <f t="shared" si="53"/>
+        <v>0.45205479452054798</v>
+      </c>
+      <c r="V56" s="1">
+        <f t="shared" si="54"/>
+        <v>6.5438999999999998</v>
+      </c>
+      <c r="W56" s="3">
+        <f t="shared" si="55"/>
+        <v>3767.0255527728282</v>
+      </c>
+      <c r="X56" s="5">
+        <f t="shared" si="56"/>
+        <v>0.61056129505333945</v>
+      </c>
+      <c r="Y56" s="5">
+        <f t="shared" si="63"/>
+        <v>2.114782608695652</v>
+      </c>
+      <c r="Z56">
+        <f t="shared" si="64"/>
+        <v>0.19965277777777779</v>
+      </c>
+      <c r="AA56">
+        <f t="shared" si="65"/>
+        <v>17.96875</v>
+      </c>
+    </row>
+    <row r="57" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A57" s="8">
+        <v>40923</v>
+      </c>
+      <c r="C57">
+        <v>45</v>
+      </c>
+      <c r="D57" s="10">
+        <v>0.99</v>
+      </c>
+      <c r="E57" s="10">
+        <v>44</v>
+      </c>
+      <c r="F57" s="10">
+        <v>40</v>
+      </c>
+      <c r="H57">
+        <v>19</v>
+      </c>
+      <c r="I57">
+        <v>2500</v>
+      </c>
+      <c r="J57" s="2">
+        <f t="shared" si="46"/>
+        <v>131.57894736842104</v>
+      </c>
+      <c r="K57">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="L57" s="3">
+        <v>4</v>
+      </c>
+      <c r="M57" s="10">
+        <v>18</v>
+      </c>
+      <c r="N57">
+        <f t="shared" si="61"/>
+        <v>258</v>
+      </c>
+      <c r="O57" s="1">
+        <f t="shared" si="62"/>
+        <v>9.6899224806201545</v>
+      </c>
+      <c r="P57">
+        <f t="shared" si="66"/>
+        <v>0</v>
+      </c>
+      <c r="Q57" s="2">
+        <f t="shared" si="67"/>
+        <v>0</v>
+      </c>
+      <c r="R57" s="5">
+        <f t="shared" si="68"/>
+        <v>0</v>
+      </c>
+      <c r="S57" s="4">
+        <f t="shared" si="69"/>
+        <v>0</v>
+      </c>
+      <c r="T57" s="5">
+        <f t="shared" si="60"/>
+        <v>8.014931927975405E-2</v>
+      </c>
+      <c r="U57" s="5">
+        <f t="shared" si="53"/>
+        <v>0.45205479452054798</v>
+      </c>
+      <c r="V57" s="1">
+        <f t="shared" si="54"/>
+        <v>6.5438999999999998</v>
+      </c>
+      <c r="W57" s="3">
+        <f t="shared" si="55"/>
+        <v>3767.0255527728282</v>
+      </c>
+      <c r="X57" s="5">
+        <f t="shared" si="56"/>
+        <v>0.66365358157971688</v>
+      </c>
+      <c r="Y57" s="5">
+        <f t="shared" si="63"/>
+        <v>1.9608000000000001</v>
+      </c>
+      <c r="Z57">
+        <f t="shared" si="64"/>
+        <v>0.21533161068044787</v>
+      </c>
+      <c r="AA57">
+        <f t="shared" si="65"/>
+        <v>17.618040873854824</v>
+      </c>
+    </row>
+    <row r="58" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A58" s="8">
+        <v>40923</v>
+      </c>
+      <c r="C58">
+        <v>45</v>
+      </c>
+      <c r="D58" s="10">
+        <v>0.99</v>
+      </c>
+      <c r="E58" s="10">
+        <v>44</v>
+      </c>
+      <c r="F58" s="10">
+        <v>40</v>
+      </c>
+      <c r="H58">
+        <v>19</v>
+      </c>
+      <c r="I58">
+        <v>2600</v>
+      </c>
+      <c r="J58" s="2">
+        <f t="shared" si="46"/>
+        <v>136.84210526315789</v>
+      </c>
+      <c r="K58">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="L58" s="3">
+        <v>4</v>
+      </c>
+      <c r="M58" s="10">
+        <v>53</v>
+      </c>
+      <c r="N58">
+        <f t="shared" si="61"/>
+        <v>293</v>
+      </c>
+      <c r="O58" s="1">
+        <f t="shared" si="62"/>
+        <v>8.8737201365187719</v>
+      </c>
+      <c r="P58">
+        <f t="shared" si="66"/>
+        <v>0</v>
+      </c>
+      <c r="Q58" s="2">
+        <f t="shared" si="67"/>
+        <v>0</v>
+      </c>
+      <c r="R58" s="5">
+        <f t="shared" si="68"/>
+        <v>0</v>
+      </c>
+      <c r="S58" s="4">
+        <f t="shared" si="69"/>
+        <v>0</v>
+      </c>
+      <c r="T58" s="5">
+        <f t="shared" si="60"/>
+        <v>8.014931927975405E-2</v>
+      </c>
+      <c r="U58" s="5">
+        <f t="shared" si="53"/>
+        <v>0.45205479452054798</v>
+      </c>
+      <c r="V58" s="1">
+        <f t="shared" si="54"/>
+        <v>6.5438999999999998</v>
+      </c>
+      <c r="W58" s="3">
+        <f t="shared" si="55"/>
+        <v>3767.0255527728282</v>
+      </c>
+      <c r="X58" s="5">
+        <f t="shared" si="56"/>
+        <v>0.69019972484290548</v>
+      </c>
+      <c r="Y58" s="5">
+        <f t="shared" si="63"/>
+        <v>2.1411538461538462</v>
+      </c>
+      <c r="Z58">
+        <f t="shared" si="64"/>
+        <v>0.19719378081152827</v>
+      </c>
+      <c r="AA58">
+        <f t="shared" si="65"/>
+        <v>16.134036611852313</v>
+      </c>
+    </row>
+    <row r="59" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A59" s="8">
+        <v>40895</v>
+      </c>
+      <c r="C59">
+        <v>45</v>
+      </c>
+      <c r="D59" s="10">
+        <v>0.7</v>
+      </c>
+      <c r="H59">
+        <v>14.5</v>
+      </c>
+      <c r="I59">
+        <v>1900</v>
+      </c>
+      <c r="J59" s="2">
+        <f t="shared" si="46"/>
+        <v>131.0344827586207</v>
+      </c>
+      <c r="K59">
+        <v>0.6</v>
+      </c>
+      <c r="L59" s="3">
+        <v>4</v>
+      </c>
+      <c r="M59" s="10">
+        <v>28</v>
+      </c>
+      <c r="N59">
+        <f t="shared" si="61"/>
+        <v>268</v>
+      </c>
+      <c r="O59" s="1">
+        <f t="shared" si="62"/>
+        <v>7.08955223880597</v>
+      </c>
+      <c r="P59">
+        <f t="shared" si="66"/>
+        <v>0</v>
+      </c>
+      <c r="Q59" s="2">
+        <f t="shared" si="67"/>
+        <v>0</v>
+      </c>
+      <c r="R59" s="5">
+        <f t="shared" si="68"/>
+        <v>0</v>
+      </c>
+      <c r="S59" s="4">
+        <f t="shared" si="69"/>
+        <v>0</v>
+      </c>
+      <c r="T59" s="5">
+        <f t="shared" si="60"/>
+        <v>9.834368530020704E-2</v>
+      </c>
+      <c r="U59" s="5">
+        <f t="shared" si="53"/>
+        <v>0.36842105263157893</v>
+      </c>
+      <c r="V59" s="1">
+        <f t="shared" si="54"/>
+        <v>4.6269999999999998</v>
+      </c>
+      <c r="W59" s="3">
+        <f t="shared" si="55"/>
+        <v>2986.6803549575679</v>
+      </c>
+      <c r="X59" s="5">
+        <f t="shared" si="56"/>
+        <v>0.63615779868984124</v>
+      </c>
+      <c r="Y59" s="5">
+        <f t="shared" si="63"/>
+        <v>2.0452631578947367</v>
+      </c>
+      <c r="Z59">
+        <f t="shared" si="64"/>
+        <v>0.15754560530679934</v>
+      </c>
+      <c r="AA59">
+        <f t="shared" si="65"/>
+        <v>11.815920398009951</v>
+      </c>
+    </row>
+    <row r="60" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A60" s="8">
+        <v>40895</v>
+      </c>
+      <c r="C60">
+        <v>45</v>
+      </c>
+      <c r="D60" s="10">
+        <v>0.9</v>
+      </c>
+      <c r="E60" s="10">
+        <v>39</v>
+      </c>
+      <c r="F60" s="10">
+        <v>40</v>
+      </c>
+      <c r="H60">
+        <v>17</v>
+      </c>
+      <c r="I60">
+        <v>2200</v>
+      </c>
+      <c r="J60" s="2">
+        <f t="shared" si="46"/>
+        <v>129.41176470588235</v>
+      </c>
+      <c r="K60">
+        <v>0.7</v>
+      </c>
+      <c r="L60" s="3">
+        <v>4</v>
+      </c>
+      <c r="M60" s="10">
+        <v>31</v>
+      </c>
+      <c r="N60">
+        <f t="shared" si="61"/>
+        <v>271</v>
+      </c>
+      <c r="O60" s="1">
+        <f t="shared" si="62"/>
+        <v>8.1180811808118083</v>
+      </c>
+      <c r="P60">
+        <f t="shared" si="66"/>
+        <v>0</v>
+      </c>
+      <c r="Q60" s="2">
+        <f t="shared" si="67"/>
+        <v>0</v>
+      </c>
+      <c r="R60" s="5">
+        <f t="shared" si="68"/>
+        <v>0</v>
+      </c>
+      <c r="S60" s="4">
+        <f t="shared" si="69"/>
+        <v>0</v>
+      </c>
+      <c r="T60" s="5">
+        <f t="shared" si="60"/>
+        <v>8.4541062801932368E-2</v>
+      </c>
+      <c r="U60" s="5">
+        <f t="shared" si="53"/>
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="V60" s="1">
+        <f t="shared" si="54"/>
+        <v>5.9490000000000007</v>
+      </c>
+      <c r="W60" s="3">
+        <f t="shared" si="55"/>
+        <v>3343.7814901922375</v>
+      </c>
+      <c r="X60" s="5">
+        <f t="shared" si="56"/>
+        <v>0.65793772902113878</v>
+      </c>
+      <c r="Y60" s="5">
+        <f t="shared" si="63"/>
+        <v>2.0940909090909092</v>
+      </c>
+      <c r="Z60">
+        <f t="shared" si="64"/>
+        <v>0.18040180401804018</v>
+      </c>
+      <c r="AA60">
+        <f t="shared" si="65"/>
+        <v>11.597258829731155</v>
+      </c>
+    </row>
+    <row r="61" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="E61" s="10"/>
+      <c r="F61" s="10"/>
+    </row>
+    <row r="62" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>29</v>
+      </c>
+      <c r="B62">
+        <v>27.6</v>
+      </c>
+    </row>
+    <row r="63" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A63" s="8">
+        <v>40432</v>
+      </c>
+      <c r="C63">
+        <v>45</v>
+      </c>
+      <c r="D63">
+        <v>0.83</v>
+      </c>
+      <c r="E63">
+        <v>39</v>
+      </c>
+      <c r="F63">
+        <v>40</v>
+      </c>
+      <c r="H63">
+        <v>17</v>
+      </c>
+      <c r="I63">
+        <v>2650</v>
+      </c>
+      <c r="J63" s="2">
+        <f t="shared" ref="J63:J68" si="70">I63/H63</f>
+        <v>155.88235294117646</v>
+      </c>
+      <c r="K63">
+        <v>0.9</v>
+      </c>
+      <c r="L63" s="3">
+        <v>5</v>
+      </c>
+      <c r="M63">
+        <v>46</v>
+      </c>
+      <c r="N63">
+        <f t="shared" ref="N63:N68" si="71">L63*60+M63</f>
+        <v>346</v>
+      </c>
+      <c r="O63" s="1">
+        <f t="shared" ref="O63:O68" si="72">I63/N63</f>
+        <v>7.6589595375722546</v>
+      </c>
+      <c r="P63">
+        <f t="shared" ref="P63:P68" si="73">G63*H63</f>
+        <v>0</v>
+      </c>
+      <c r="Q63" s="2">
+        <f t="shared" ref="Q63:Q68" si="74">P63/D63</f>
+        <v>0</v>
+      </c>
+      <c r="R63" s="5">
+        <f t="shared" ref="R63:R68" si="75">P63/I63</f>
+        <v>0</v>
+      </c>
+      <c r="S63" s="4">
+        <f t="shared" ref="S63:S68" si="76">R63/I63</f>
+        <v>0</v>
+      </c>
+      <c r="T63" s="5">
+        <f>$B$62/(483*U63)</f>
+        <v>0.13975903614457832</v>
+      </c>
+      <c r="U63" s="5">
+        <f t="shared" ref="U63:U68" si="77">D63/(1.2+D63)</f>
+        <v>0.40886699507389163</v>
+      </c>
+      <c r="V63" s="1">
+        <f t="shared" ref="V63:V68" si="78">6.61 * D63</f>
+        <v>5.4863</v>
+      </c>
+      <c r="W63" s="3">
+        <f t="shared" ref="W63:W68" si="79">45.257*H63/SQRT(D63/H63)</f>
+        <v>3481.9304970705716</v>
+      </c>
+      <c r="X63" s="5">
+        <f t="shared" ref="X63:X68" si="80">I63/W63</f>
+        <v>0.76107205535248512</v>
+      </c>
+      <c r="Y63" s="5">
+        <f t="shared" ref="Y63:Y68" si="81">N63/J63</f>
+        <v>2.2196226415094342</v>
+      </c>
+      <c r="Z63">
+        <f t="shared" ref="Z63:Z68" si="82">O63/C63</f>
+        <v>0.170199100834939</v>
+      </c>
+      <c r="AA63">
+        <f t="shared" ref="AA63:AA68" si="83">O63/K63</f>
+        <v>8.5099550417469487</v>
+      </c>
+    </row>
+    <row r="64" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A64" s="8">
+        <v>40496</v>
+      </c>
+      <c r="C64">
+        <v>47</v>
+      </c>
+      <c r="D64">
+        <v>1.04</v>
+      </c>
+      <c r="H64">
+        <v>18</v>
+      </c>
+      <c r="I64">
+        <v>2950</v>
+      </c>
+      <c r="J64" s="2">
+        <f t="shared" si="70"/>
+        <v>163.88888888888889</v>
+      </c>
+      <c r="K64">
+        <v>1.2</v>
+      </c>
+      <c r="L64" s="3">
+        <v>5</v>
+      </c>
+      <c r="M64">
+        <v>58</v>
+      </c>
+      <c r="N64">
+        <f t="shared" si="71"/>
+        <v>358</v>
+      </c>
+      <c r="O64" s="1">
+        <f t="shared" si="72"/>
+        <v>8.2402234636871512</v>
+      </c>
+      <c r="P64">
+        <f t="shared" si="73"/>
+        <v>0</v>
+      </c>
+      <c r="Q64" s="2">
+        <f t="shared" si="74"/>
+        <v>0</v>
+      </c>
+      <c r="R64" s="5">
+        <f t="shared" si="75"/>
+        <v>0</v>
+      </c>
+      <c r="S64" s="4">
+        <f t="shared" si="76"/>
+        <v>0</v>
+      </c>
+      <c r="T64" s="5">
+        <f>$B$62/(483*U64)</f>
+        <v>0.1230769230769231</v>
+      </c>
+      <c r="U64" s="5">
+        <f t="shared" si="77"/>
+        <v>0.46428571428571425</v>
+      </c>
+      <c r="V64" s="1">
+        <f t="shared" si="78"/>
+        <v>6.8744000000000005</v>
+      </c>
+      <c r="W64" s="3">
+        <f t="shared" si="79"/>
+        <v>3389.0490153763012</v>
+      </c>
+      <c r="X64" s="5">
+        <f t="shared" si="80"/>
+        <v>0.87045067410228893</v>
+      </c>
+      <c r="Y64" s="5">
+        <f t="shared" si="81"/>
+        <v>2.1844067796610172</v>
+      </c>
+      <c r="Z64">
+        <f t="shared" si="82"/>
+        <v>0.17532390348270535</v>
+      </c>
+      <c r="AA64">
+        <f t="shared" si="83"/>
+        <v>6.8668528864059599</v>
+      </c>
+    </row>
+    <row r="65" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A65" s="8">
+        <v>40496</v>
+      </c>
+      <c r="C65">
+        <v>47</v>
+      </c>
+      <c r="D65">
+        <v>1.04</v>
+      </c>
+      <c r="H65">
+        <v>18</v>
+      </c>
+      <c r="I65">
+        <v>3150</v>
+      </c>
+      <c r="J65" s="2">
+        <f t="shared" si="70"/>
+        <v>175</v>
+      </c>
+      <c r="K65">
+        <v>1.4</v>
+      </c>
+      <c r="L65" s="3">
+        <v>5</v>
+      </c>
+      <c r="M65">
+        <v>56</v>
+      </c>
+      <c r="N65">
+        <f t="shared" si="71"/>
+        <v>356</v>
+      </c>
+      <c r="O65" s="1">
+        <f t="shared" si="72"/>
+        <v>8.8483146067415728</v>
+      </c>
+      <c r="P65">
+        <f t="shared" si="73"/>
+        <v>0</v>
+      </c>
+      <c r="Q65" s="2">
+        <f t="shared" si="74"/>
+        <v>0</v>
+      </c>
+      <c r="R65" s="5">
+        <f t="shared" si="75"/>
+        <v>0</v>
+      </c>
+      <c r="S65" s="4">
+        <f t="shared" si="76"/>
+        <v>0</v>
+      </c>
+      <c r="T65" s="5">
+        <f>$B$62/(483*U65)</f>
+        <v>0.1230769230769231</v>
+      </c>
+      <c r="U65" s="5">
+        <f t="shared" si="77"/>
+        <v>0.46428571428571425</v>
+      </c>
+      <c r="V65" s="1">
+        <f t="shared" si="78"/>
+        <v>6.8744000000000005</v>
+      </c>
+      <c r="W65" s="3">
+        <f t="shared" si="79"/>
+        <v>3389.0490153763012</v>
+      </c>
+      <c r="X65" s="5">
+        <f t="shared" si="80"/>
+        <v>0.92946427912617291</v>
+      </c>
+      <c r="Y65" s="5">
+        <f t="shared" si="81"/>
+        <v>2.0342857142857143</v>
+      </c>
+      <c r="Z65">
+        <f t="shared" si="82"/>
+        <v>0.18826201290939518</v>
+      </c>
+      <c r="AA65">
+        <f t="shared" si="83"/>
+        <v>6.320224719101124</v>
+      </c>
+    </row>
+    <row r="66" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A66" s="8">
+        <v>40587</v>
+      </c>
+      <c r="C66">
+        <v>45</v>
+      </c>
+      <c r="D66">
+        <v>1</v>
+      </c>
+      <c r="E66">
+        <v>45</v>
+      </c>
+      <c r="F66">
+        <v>40</v>
+      </c>
+      <c r="H66">
+        <v>18.5</v>
+      </c>
+      <c r="I66">
+        <v>2500</v>
+      </c>
+      <c r="J66" s="2">
+        <f t="shared" si="70"/>
+        <v>135.13513513513513</v>
+      </c>
+      <c r="K66">
+        <v>1.8</v>
+      </c>
+      <c r="L66" s="3">
+        <v>7</v>
+      </c>
+      <c r="M66">
+        <v>3</v>
+      </c>
+      <c r="N66">
+        <f t="shared" si="71"/>
+        <v>423</v>
+      </c>
+      <c r="O66" s="1">
+        <f t="shared" si="72"/>
+        <v>5.9101654846335698</v>
+      </c>
+      <c r="P66">
+        <f t="shared" si="73"/>
+        <v>0</v>
+      </c>
+      <c r="Q66" s="2">
+        <f t="shared" si="74"/>
+        <v>0</v>
+      </c>
+      <c r="R66" s="5">
+        <f t="shared" si="75"/>
+        <v>0</v>
+      </c>
+      <c r="S66" s="4">
+        <f t="shared" si="76"/>
+        <v>0</v>
+      </c>
+      <c r="T66" s="5">
+        <f>$B$62/(483*U66)</f>
+        <v>0.12571428571428572</v>
+      </c>
+      <c r="U66" s="5">
+        <f t="shared" si="77"/>
+        <v>0.45454545454545453</v>
+      </c>
+      <c r="V66" s="1">
+        <f t="shared" si="78"/>
+        <v>6.61</v>
+      </c>
+      <c r="W66" s="3">
+        <f t="shared" si="79"/>
+        <v>3601.1677701475705</v>
+      </c>
+      <c r="X66" s="5">
+        <f t="shared" si="80"/>
+        <v>0.69421925318896038</v>
+      </c>
+      <c r="Y66" s="5">
+        <f t="shared" si="81"/>
+        <v>3.1302000000000003</v>
+      </c>
+      <c r="Z66">
+        <f t="shared" si="82"/>
+        <v>0.13133701076963489</v>
+      </c>
+      <c r="AA66">
+        <f t="shared" si="83"/>
+        <v>3.2834252692408721</v>
+      </c>
+    </row>
+    <row r="67" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A67" s="8">
+        <v>40587</v>
+      </c>
+      <c r="C67">
+        <v>47</v>
+      </c>
+      <c r="D67">
+        <v>1</v>
+      </c>
+      <c r="E67">
+        <v>45</v>
+      </c>
+      <c r="F67">
+        <v>40</v>
+      </c>
+      <c r="H67">
+        <v>18</v>
+      </c>
+      <c r="I67">
+        <v>3025</v>
+      </c>
+      <c r="J67" s="2">
+        <f t="shared" si="70"/>
+        <v>168.05555555555554</v>
+      </c>
+      <c r="K67">
+        <v>2.95</v>
+      </c>
+      <c r="L67" s="3">
+        <v>6</v>
+      </c>
+      <c r="M67">
+        <v>52</v>
+      </c>
+      <c r="N67">
+        <f t="shared" si="71"/>
+        <v>412</v>
+      </c>
+      <c r="O67" s="1">
+        <f t="shared" si="72"/>
+        <v>7.342233009708738</v>
+      </c>
+      <c r="P67">
+        <f t="shared" si="73"/>
+        <v>0</v>
+      </c>
+      <c r="Q67" s="2">
+        <f t="shared" si="74"/>
+        <v>0</v>
+      </c>
+      <c r="R67" s="5">
+        <f t="shared" si="75"/>
+        <v>0</v>
+      </c>
+      <c r="S67" s="4">
+        <f t="shared" si="76"/>
+        <v>0</v>
+      </c>
+      <c r="T67" s="5">
+        <f>$B$62/(483*U67)</f>
+        <v>0.12571428571428572</v>
+      </c>
+      <c r="U67" s="5">
+        <f t="shared" si="77"/>
+        <v>0.45454545454545453</v>
+      </c>
+      <c r="V67" s="1">
+        <f t="shared" si="78"/>
+        <v>6.61</v>
+      </c>
+      <c r="W67" s="3">
+        <f t="shared" si="79"/>
+        <v>3456.1654123852345</v>
+      </c>
+      <c r="X67" s="5">
+        <f t="shared" si="80"/>
+        <v>0.87524746042531842</v>
+      </c>
+      <c r="Y67" s="5">
+        <f t="shared" si="81"/>
+        <v>2.4515702479338843</v>
+      </c>
+      <c r="Z67">
+        <f t="shared" si="82"/>
+        <v>0.15621772361082423</v>
+      </c>
+      <c r="AA67">
+        <f t="shared" si="83"/>
+        <v>2.4888925456639788</v>
+      </c>
+    </row>
+    <row r="68" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A68" s="8">
+        <v>40811</v>
+      </c>
+      <c r="C68">
+        <v>45</v>
+      </c>
+      <c r="D68">
+        <v>0.87</v>
+      </c>
+      <c r="E68">
+        <v>41</v>
+      </c>
+      <c r="F68">
+        <v>42</v>
+      </c>
+      <c r="H68">
+        <v>18</v>
+      </c>
+      <c r="I68">
+        <v>3450</v>
+      </c>
+      <c r="J68" s="2">
+        <f t="shared" si="70"/>
+        <v>191.66666666666666</v>
+      </c>
+      <c r="K68">
+        <v>1.5</v>
+      </c>
+      <c r="L68" s="3">
+        <v>6</v>
+      </c>
+      <c r="M68">
+        <v>42</v>
+      </c>
+      <c r="N68">
+        <f t="shared" si="71"/>
+        <v>402</v>
+      </c>
+      <c r="O68" s="1">
+        <f t="shared" si="72"/>
+        <v>8.5820895522388057</v>
+      </c>
+      <c r="P68">
+        <f t="shared" si="73"/>
+        <v>0</v>
+      </c>
+      <c r="Q68" s="2">
+        <f t="shared" si="74"/>
+        <v>0</v>
+      </c>
+      <c r="R68" s="5">
+        <f t="shared" si="75"/>
+        <v>0</v>
+      </c>
+      <c r="S68" s="4">
+        <f t="shared" si="76"/>
+        <v>0</v>
+      </c>
+      <c r="T68" s="5">
+        <f>$B$362/(483*U68)</f>
+        <v>0</v>
+      </c>
+      <c r="U68" s="5">
+        <f t="shared" si="77"/>
+        <v>0.4202898550724638</v>
+      </c>
+      <c r="V68" s="1">
+        <f t="shared" si="78"/>
+        <v>5.7507000000000001</v>
+      </c>
+      <c r="W68" s="3">
+        <f t="shared" si="79"/>
+        <v>3705.3982610910466</v>
+      </c>
+      <c r="X68" s="5">
+        <f t="shared" si="80"/>
+        <v>0.93107400524988504</v>
+      </c>
+      <c r="Y68" s="5">
+        <f t="shared" si="81"/>
+        <v>2.0973913043478261</v>
+      </c>
+      <c r="Z68">
+        <f t="shared" si="82"/>
+        <v>0.19071310116086235</v>
+      </c>
+      <c r="AA68">
+        <f t="shared" si="83"/>
+        <v>5.7213930348258701</v>
+      </c>
+    </row>
+    <row r="70" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>30</v>
+      </c>
+      <c r="B70">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="71" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A71" s="8">
+        <v>39550</v>
+      </c>
+      <c r="C71">
+        <v>47</v>
+      </c>
+      <c r="D71">
+        <v>0.81</v>
+      </c>
+      <c r="E71">
+        <v>39</v>
+      </c>
+      <c r="F71">
+        <v>40</v>
+      </c>
+      <c r="H71">
+        <v>16.5</v>
+      </c>
+      <c r="I71">
+        <v>2700</v>
+      </c>
+      <c r="J71" s="2">
+        <f t="shared" ref="J71:J77" si="84">I71/H71</f>
+        <v>163.63636363636363</v>
+      </c>
+      <c r="K71">
+        <v>1</v>
+      </c>
+      <c r="L71" s="3">
+        <v>5</v>
+      </c>
+      <c r="M71">
+        <v>10</v>
+      </c>
+      <c r="N71">
+        <f>L71*60+M71</f>
+        <v>310</v>
+      </c>
+      <c r="O71" s="1">
+        <f>I71/N71</f>
+        <v>8.7096774193548381</v>
+      </c>
+      <c r="P71">
+        <f>G71*H71</f>
+        <v>0</v>
+      </c>
+      <c r="Q71" s="2">
+        <f>P71/D71</f>
+        <v>0</v>
+      </c>
+      <c r="R71" s="5">
+        <f>P71/I71</f>
+        <v>0</v>
+      </c>
+      <c r="S71" s="4">
+        <f>R71/I71</f>
+        <v>0</v>
+      </c>
+      <c r="T71" s="5">
+        <f>$B$2/(483*U71)</f>
+        <v>1.0172532781228432</v>
+      </c>
+      <c r="U71" s="5">
+        <f>D71/(1.2+D71)</f>
+        <v>0.40298507462686572</v>
+      </c>
+      <c r="V71" s="1">
+        <f t="shared" ref="V71:V74" si="85">6.61 * D71</f>
+        <v>5.3541000000000007</v>
+      </c>
+      <c r="W71" s="3">
+        <f>45.257*H71/SQRT(D71/H71)</f>
+        <v>3370.304722387255</v>
+      </c>
+      <c r="X71" s="5">
+        <f>I71/W71</f>
+        <v>0.80111450518561289</v>
+      </c>
+      <c r="Y71" s="5">
+        <f>N71/J71</f>
+        <v>1.8944444444444446</v>
+      </c>
+      <c r="Z71">
+        <f>O71/C71</f>
+        <v>0.18531228551818804</v>
+      </c>
+      <c r="AA71">
+        <f>O71/K71</f>
+        <v>8.7096774193548381</v>
+      </c>
+    </row>
+    <row r="72" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A72" s="8">
+        <v>39550</v>
+      </c>
+      <c r="C72">
+        <v>47</v>
+      </c>
+      <c r="D72">
+        <v>0.81</v>
+      </c>
+      <c r="E72">
+        <v>39</v>
+      </c>
+      <c r="F72">
+        <v>40</v>
+      </c>
+      <c r="H72">
+        <v>16.5</v>
+      </c>
+      <c r="I72">
+        <v>2900</v>
+      </c>
+      <c r="J72" s="2">
+        <f t="shared" si="84"/>
+        <v>175.75757575757575</v>
+      </c>
+      <c r="K72">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="L72" s="3">
+        <v>5</v>
+      </c>
+      <c r="M72">
+        <v>34</v>
+      </c>
+      <c r="N72">
+        <f t="shared" ref="N72:N77" si="86">L72*60+M72</f>
+        <v>334</v>
+      </c>
+      <c r="O72" s="1">
+        <f t="shared" ref="O72:O77" si="87">I72/N72</f>
+        <v>8.682634730538922</v>
+      </c>
+      <c r="P72">
+        <f t="shared" ref="P72:P77" si="88">G72*H72</f>
+        <v>0</v>
+      </c>
+      <c r="Q72" s="2">
+        <f t="shared" ref="Q72:Q77" si="89">P72/D72</f>
+        <v>0</v>
+      </c>
+      <c r="R72" s="5">
+        <f t="shared" ref="R72:R77" si="90">P72/I72</f>
+        <v>0</v>
+      </c>
+      <c r="S72" s="4">
+        <f t="shared" ref="S72:S77" si="91">R72/I72</f>
+        <v>0</v>
+      </c>
+      <c r="T72" s="5">
+        <f t="shared" ref="T72:T77" si="92">$B$2/(483*U72)</f>
+        <v>1.0172532781228432</v>
+      </c>
+      <c r="U72" s="5">
+        <f t="shared" ref="U72:U77" si="93">D72/(1.2+D72)</f>
+        <v>0.40298507462686572</v>
+      </c>
+      <c r="V72" s="1">
+        <f t="shared" ref="V72:V77" si="94">6.61 * D72</f>
+        <v>5.3541000000000007</v>
+      </c>
+      <c r="W72" s="3">
+        <f t="shared" ref="W72:W77" si="95">45.257*H72/SQRT(D72/H72)</f>
+        <v>3370.304722387255</v>
+      </c>
+      <c r="X72" s="5">
+        <f t="shared" ref="X72:X77" si="96">I72/W72</f>
+        <v>0.86045632038454711</v>
+      </c>
+      <c r="Y72" s="5">
+        <f t="shared" ref="Y72:Y77" si="97">N72/J72</f>
+        <v>1.9003448275862069</v>
+      </c>
+      <c r="Z72">
+        <f t="shared" ref="Z72:Z77" si="98">O72/C72</f>
+        <v>0.18473690916040258</v>
+      </c>
+      <c r="AA72">
+        <f t="shared" ref="AA72:AA77" si="99">O72/K72</f>
+        <v>7.8933043004899286</v>
+      </c>
+    </row>
+    <row r="73" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A73" s="8">
+        <v>39916</v>
+      </c>
+      <c r="C73">
+        <v>45</v>
+      </c>
+      <c r="D73">
+        <v>0.81</v>
+      </c>
+      <c r="E73">
+        <v>39</v>
+      </c>
+      <c r="F73">
+        <v>40</v>
+      </c>
+      <c r="H73">
+        <v>16.5</v>
+      </c>
+      <c r="I73">
+        <v>2725</v>
+      </c>
+      <c r="J73" s="2">
+        <f t="shared" si="84"/>
+        <v>165.15151515151516</v>
+      </c>
+      <c r="K73">
+        <v>0.75</v>
+      </c>
+      <c r="L73" s="3">
+        <v>5</v>
+      </c>
+      <c r="M73">
+        <v>32</v>
+      </c>
+      <c r="N73">
+        <f t="shared" si="86"/>
+        <v>332</v>
+      </c>
+      <c r="O73" s="1">
+        <f t="shared" si="87"/>
+        <v>8.2078313253012052</v>
+      </c>
+      <c r="P73">
+        <f t="shared" si="88"/>
+        <v>0</v>
+      </c>
+      <c r="Q73" s="2">
+        <f t="shared" si="89"/>
+        <v>0</v>
+      </c>
+      <c r="R73" s="5">
+        <f t="shared" si="90"/>
+        <v>0</v>
+      </c>
+      <c r="S73" s="4">
+        <f t="shared" si="91"/>
+        <v>0</v>
+      </c>
+      <c r="T73" s="5">
+        <f t="shared" si="92"/>
+        <v>1.0172532781228432</v>
+      </c>
+      <c r="U73" s="5">
+        <f t="shared" si="93"/>
+        <v>0.40298507462686572</v>
+      </c>
+      <c r="V73" s="1">
+        <f t="shared" si="94"/>
+        <v>5.3541000000000007</v>
+      </c>
+      <c r="W73" s="3">
+        <f t="shared" si="95"/>
+        <v>3370.304722387255</v>
+      </c>
+      <c r="X73" s="5">
+        <f t="shared" si="96"/>
+        <v>0.80853223208547964</v>
+      </c>
+      <c r="Y73" s="5">
+        <f t="shared" si="97"/>
+        <v>2.0102752293577981</v>
+      </c>
+      <c r="Z73">
+        <f t="shared" si="98"/>
+        <v>0.18239625167336013</v>
+      </c>
+      <c r="AA73">
+        <f t="shared" si="99"/>
+        <v>10.943775100401608</v>
+      </c>
+    </row>
+    <row r="74" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A74" s="8">
+        <v>40642</v>
+      </c>
+      <c r="C74" s="7">
+        <v>45</v>
+      </c>
+      <c r="D74">
+        <v>0.72</v>
+      </c>
+      <c r="E74">
+        <v>37</v>
+      </c>
+      <c r="F74">
+        <v>40</v>
+      </c>
+      <c r="H74">
+        <v>15.5</v>
+      </c>
+      <c r="I74">
+        <v>2425</v>
+      </c>
+      <c r="J74" s="2">
+        <f t="shared" si="84"/>
+        <v>156.45161290322579</v>
+      </c>
+      <c r="K74">
+        <v>0.7</v>
+      </c>
+      <c r="L74" s="3">
+        <v>4</v>
+      </c>
+      <c r="M74">
+        <v>23</v>
+      </c>
+      <c r="N74">
+        <f t="shared" si="86"/>
+        <v>263</v>
+      </c>
+      <c r="O74" s="1">
+        <f t="shared" si="87"/>
+        <v>9.2205323193916353</v>
+      </c>
+      <c r="P74">
+        <f t="shared" si="88"/>
+        <v>0</v>
+      </c>
+      <c r="Q74" s="2">
+        <f t="shared" si="89"/>
+        <v>0</v>
+      </c>
+      <c r="R74" s="5">
+        <f t="shared" si="90"/>
+        <v>0</v>
+      </c>
+      <c r="S74" s="4">
+        <f t="shared" si="91"/>
+        <v>0</v>
+      </c>
+      <c r="T74" s="5">
+        <f t="shared" si="92"/>
+        <v>1.0931677018633541</v>
+      </c>
+      <c r="U74" s="5">
+        <f t="shared" si="93"/>
+        <v>0.375</v>
+      </c>
+      <c r="V74" s="1">
+        <f t="shared" si="94"/>
+        <v>4.7591999999999999</v>
+      </c>
+      <c r="W74" s="3">
+        <f t="shared" si="95"/>
+        <v>3254.7456936777276</v>
+      </c>
+      <c r="X74" s="5">
+        <f t="shared" si="96"/>
+        <v>0.74506589092675035</v>
+      </c>
+      <c r="Y74" s="5">
+        <f t="shared" si="97"/>
+        <v>1.6810309278350517</v>
+      </c>
+      <c r="Z74">
+        <f t="shared" si="98"/>
+        <v>0.20490071820870301</v>
+      </c>
+      <c r="AA74">
+        <f t="shared" si="99"/>
+        <v>13.172189027702338</v>
+      </c>
+    </row>
+    <row r="75" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A75" s="8">
+        <v>40642</v>
+      </c>
+      <c r="C75">
+        <v>45</v>
+      </c>
+      <c r="D75">
+        <v>0.72</v>
+      </c>
+      <c r="E75">
+        <v>37</v>
+      </c>
+      <c r="F75">
+        <v>40</v>
+      </c>
+      <c r="H75">
+        <v>15.5</v>
+      </c>
+      <c r="I75">
+        <v>2500</v>
+      </c>
+      <c r="J75" s="2">
+        <f t="shared" si="84"/>
+        <v>161.29032258064515</v>
+      </c>
+      <c r="K75">
+        <v>0.7</v>
+      </c>
+      <c r="L75" s="3">
+        <v>4</v>
+      </c>
+      <c r="M75">
+        <v>59</v>
+      </c>
+      <c r="N75">
+        <f t="shared" si="86"/>
+        <v>299</v>
+      </c>
+      <c r="O75" s="1">
+        <f t="shared" si="87"/>
+        <v>8.3612040133779271</v>
+      </c>
+      <c r="P75">
+        <f t="shared" si="88"/>
+        <v>0</v>
+      </c>
+      <c r="Q75" s="2">
+        <f t="shared" si="89"/>
+        <v>0</v>
+      </c>
+      <c r="R75" s="5">
+        <f t="shared" si="90"/>
+        <v>0</v>
+      </c>
+      <c r="S75" s="4">
+        <f t="shared" si="91"/>
+        <v>0</v>
+      </c>
+      <c r="T75" s="5">
+        <f t="shared" si="92"/>
+        <v>1.0931677018633541</v>
+      </c>
+      <c r="U75" s="5">
+        <f t="shared" si="93"/>
+        <v>0.375</v>
+      </c>
+      <c r="V75" s="1">
+        <f t="shared" si="94"/>
+        <v>4.7591999999999999</v>
+      </c>
+      <c r="W75" s="3">
+        <f t="shared" si="95"/>
+        <v>3254.7456936777276</v>
+      </c>
+      <c r="X75" s="5">
+        <f t="shared" si="96"/>
+        <v>0.76810916590386624</v>
+      </c>
+      <c r="Y75" s="5">
+        <f t="shared" si="97"/>
+        <v>1.8538000000000001</v>
+      </c>
+      <c r="Z75">
+        <f t="shared" si="98"/>
+        <v>0.18580453363062061</v>
+      </c>
+      <c r="AA75">
+        <f t="shared" si="99"/>
+        <v>11.944577161968468</v>
+      </c>
+    </row>
+    <row r="76" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A76" s="8">
+        <v>40642</v>
+      </c>
+      <c r="C76">
+        <v>45</v>
+      </c>
+      <c r="D76">
+        <v>0.72</v>
+      </c>
+      <c r="E76">
+        <v>37</v>
+      </c>
+      <c r="F76">
+        <v>40</v>
+      </c>
+      <c r="H76">
+        <v>15.5</v>
+      </c>
+      <c r="I76">
+        <v>2550</v>
+      </c>
+      <c r="J76" s="2">
+        <f t="shared" si="84"/>
+        <v>164.51612903225808</v>
+      </c>
+      <c r="K76">
+        <v>0.7</v>
+      </c>
+      <c r="L76" s="3">
+        <v>5</v>
+      </c>
+      <c r="M76">
+        <v>3</v>
+      </c>
+      <c r="N76">
+        <f t="shared" si="86"/>
+        <v>303</v>
+      </c>
+      <c r="O76" s="1">
+        <f t="shared" si="87"/>
+        <v>8.4158415841584162</v>
+      </c>
+      <c r="P76">
+        <f t="shared" si="88"/>
+        <v>0</v>
+      </c>
+      <c r="Q76" s="2">
+        <f t="shared" si="89"/>
+        <v>0</v>
+      </c>
+      <c r="R76" s="5">
+        <f t="shared" si="90"/>
+        <v>0</v>
+      </c>
+      <c r="S76" s="4">
+        <f t="shared" si="91"/>
+        <v>0</v>
+      </c>
+      <c r="T76" s="5">
+        <f t="shared" si="92"/>
+        <v>1.0931677018633541</v>
+      </c>
+      <c r="U76" s="5">
+        <f t="shared" si="93"/>
+        <v>0.375</v>
+      </c>
+      <c r="V76" s="1">
+        <f t="shared" si="94"/>
+        <v>4.7591999999999999</v>
+      </c>
+      <c r="W76" s="3">
+        <f t="shared" si="95"/>
+        <v>3254.7456936777276</v>
+      </c>
+      <c r="X76" s="5">
+        <f t="shared" si="96"/>
+        <v>0.78347134922194361</v>
+      </c>
+      <c r="Y76" s="5">
+        <f t="shared" si="97"/>
+        <v>1.8417647058823527</v>
+      </c>
+      <c r="Z76">
+        <f t="shared" si="98"/>
+        <v>0.18701870187018702</v>
+      </c>
+      <c r="AA76">
+        <f t="shared" si="99"/>
+        <v>12.022630834512023</v>
+      </c>
+    </row>
+    <row r="77" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A77" s="8">
+        <v>40642</v>
+      </c>
+      <c r="C77">
+        <v>45</v>
+      </c>
+      <c r="D77">
+        <v>0.72</v>
+      </c>
+      <c r="E77">
+        <v>37</v>
+      </c>
+      <c r="F77">
+        <v>40</v>
+      </c>
+      <c r="H77">
+        <v>15.5</v>
+      </c>
+      <c r="I77">
+        <v>2525</v>
+      </c>
+      <c r="J77" s="2">
+        <f t="shared" si="84"/>
+        <v>162.90322580645162</v>
+      </c>
+      <c r="K77">
+        <v>0.7</v>
+      </c>
+      <c r="L77" s="3">
+        <v>4</v>
+      </c>
+      <c r="M77">
+        <v>54</v>
+      </c>
+      <c r="N77">
+        <f t="shared" si="86"/>
+        <v>294</v>
+      </c>
+      <c r="O77" s="1">
+        <f t="shared" si="87"/>
+        <v>8.5884353741496593</v>
+      </c>
+      <c r="P77">
+        <f t="shared" si="88"/>
+        <v>0</v>
+      </c>
+      <c r="Q77" s="2">
+        <f t="shared" si="89"/>
+        <v>0</v>
+      </c>
+      <c r="R77" s="5">
+        <f t="shared" si="90"/>
+        <v>0</v>
+      </c>
+      <c r="S77" s="4">
+        <f t="shared" si="91"/>
+        <v>0</v>
+      </c>
+      <c r="T77" s="5">
+        <f t="shared" si="92"/>
+        <v>1.0931677018633541</v>
+      </c>
+      <c r="U77" s="5">
+        <f t="shared" si="93"/>
+        <v>0.375</v>
+      </c>
+      <c r="V77" s="1">
+        <f t="shared" si="94"/>
+        <v>4.7591999999999999</v>
+      </c>
+      <c r="W77" s="3">
+        <f t="shared" si="95"/>
+        <v>3254.7456936777276</v>
+      </c>
+      <c r="X77" s="5">
+        <f t="shared" si="96"/>
+        <v>0.77579025756290498</v>
+      </c>
+      <c r="Y77" s="5">
+        <f t="shared" si="97"/>
+        <v>1.8047524752475248</v>
+      </c>
+      <c r="Z77">
+        <f t="shared" si="98"/>
+        <v>0.19085411942554797</v>
+      </c>
+      <c r="AA77">
+        <f t="shared" si="99"/>
+        <v>12.269193391642371</v>
+      </c>
+    </row>
+    <row r="79" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="80" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A80" s="8">
+        <v>38393</v>
+      </c>
+      <c r="C80">
+        <v>45</v>
+      </c>
+      <c r="D80">
+        <v>0.61</v>
+      </c>
+      <c r="E80">
+        <v>35</v>
+      </c>
+      <c r="F80">
+        <v>40</v>
+      </c>
+      <c r="H80">
+        <v>14.5</v>
+      </c>
+      <c r="I80">
+        <v>1650</v>
+      </c>
+      <c r="J80" s="2">
+        <f t="shared" ref="J80:J83" si="100">I80/H80</f>
+        <v>113.79310344827586</v>
+      </c>
+      <c r="K80">
+        <v>0.39</v>
+      </c>
+      <c r="L80" s="3">
+        <v>4</v>
+      </c>
+      <c r="M80">
+        <v>20</v>
+      </c>
+      <c r="N80">
+        <f t="shared" ref="N80:N83" si="101">L80*60+M80</f>
+        <v>260</v>
+      </c>
+      <c r="O80" s="1">
+        <f t="shared" ref="O80:O83" si="102">I80/N80</f>
+        <v>6.3461538461538458</v>
+      </c>
+      <c r="P80">
+        <f t="shared" ref="P80:P83" si="103">G80*H80</f>
+        <v>0</v>
+      </c>
+      <c r="Q80" s="2">
+        <f t="shared" ref="Q80:Q83" si="104">P80/D80</f>
+        <v>0</v>
+      </c>
+      <c r="R80" s="5">
+        <f t="shared" ref="R80:R83" si="105">P80/I80</f>
+        <v>0</v>
+      </c>
+      <c r="S80" s="4">
+        <f t="shared" ref="S80:S83" si="106">R80/I80</f>
+        <v>0</v>
+      </c>
+      <c r="T80" s="5">
+        <f t="shared" ref="T80:T83" si="107">$B$2/(483*U80)</f>
+        <v>1.2163730780979534</v>
+      </c>
+      <c r="U80" s="5">
+        <f t="shared" ref="U80:U83" si="108">D80/(1.2+D80)</f>
+        <v>0.33701657458563533</v>
+      </c>
+      <c r="V80" s="1">
+        <f t="shared" ref="V80:V83" si="109">6.61 * D80</f>
+        <v>4.0320999999999998</v>
+      </c>
+      <c r="W80" s="3">
+        <f t="shared" ref="W80:W83" si="110">45.257*H80/SQRT(D80/H80)</f>
+        <v>3199.4317322992915</v>
+      </c>
+      <c r="X80" s="5">
+        <f t="shared" ref="X80:X83" si="111">I80/W80</f>
+        <v>0.51571658283648303</v>
+      </c>
+      <c r="Y80" s="5">
+        <f t="shared" ref="Y80:Y83" si="112">N80/J80</f>
+        <v>2.2848484848484851</v>
+      </c>
+      <c r="Z80">
+        <f t="shared" ref="Z80:Z83" si="113">O80/C80</f>
+        <v>0.14102564102564102</v>
+      </c>
+      <c r="AA80">
+        <f t="shared" ref="AA80:AA83" si="114">O80/K80</f>
+        <v>16.272189349112423</v>
+      </c>
+    </row>
+    <row r="81" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A81" s="8">
+        <v>38429</v>
+      </c>
+      <c r="C81">
+        <v>45</v>
+      </c>
+      <c r="D81">
+        <v>0.42</v>
+      </c>
+      <c r="E81">
+        <v>30</v>
+      </c>
+      <c r="F81">
+        <v>42</v>
+      </c>
+      <c r="H81">
+        <v>11</v>
+      </c>
+      <c r="I81">
+        <v>1735</v>
+      </c>
+      <c r="J81" s="2">
+        <f t="shared" si="100"/>
+        <v>157.72727272727272</v>
+      </c>
+      <c r="K81">
+        <v>0.5</v>
+      </c>
+      <c r="L81" s="3">
+        <v>4</v>
+      </c>
+      <c r="M81">
+        <v>24</v>
+      </c>
+      <c r="N81">
+        <f t="shared" si="101"/>
+        <v>264</v>
+      </c>
+      <c r="O81" s="1">
+        <f t="shared" si="102"/>
+        <v>6.5719696969696972</v>
+      </c>
+      <c r="P81">
+        <f t="shared" si="103"/>
+        <v>0</v>
+      </c>
+      <c r="Q81" s="2">
+        <f t="shared" si="104"/>
+        <v>0</v>
+      </c>
+      <c r="R81" s="5">
+        <f t="shared" si="105"/>
+        <v>0</v>
+      </c>
+      <c r="S81" s="4">
+        <f t="shared" si="106"/>
+        <v>0</v>
+      </c>
+      <c r="T81" s="5">
+        <f t="shared" si="107"/>
+        <v>1.5811889973380657</v>
+      </c>
+      <c r="U81" s="5">
+        <f t="shared" si="108"/>
+        <v>0.25925925925925924</v>
+      </c>
+      <c r="V81" s="1">
+        <f t="shared" si="109"/>
+        <v>2.7762000000000002</v>
+      </c>
+      <c r="W81" s="3">
+        <f t="shared" si="110"/>
+        <v>2547.7108965552179</v>
+      </c>
+      <c r="X81" s="5">
+        <f t="shared" si="111"/>
+        <v>0.68100348526432442</v>
+      </c>
+      <c r="Y81" s="5">
+        <f t="shared" si="112"/>
+        <v>1.6737752161383286</v>
+      </c>
+      <c r="Z81">
+        <f t="shared" si="113"/>
+        <v>0.14604377104377106</v>
+      </c>
+      <c r="AA81">
+        <f t="shared" si="114"/>
+        <v>13.143939393939394</v>
+      </c>
+    </row>
+    <row r="82" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A82" s="8">
+        <v>38429</v>
+      </c>
+      <c r="C82">
+        <v>45</v>
+      </c>
+      <c r="D82">
+        <v>0.61</v>
+      </c>
+      <c r="E82">
+        <v>30</v>
+      </c>
+      <c r="F82">
+        <v>42</v>
+      </c>
+      <c r="H82">
+        <v>14.5</v>
+      </c>
+      <c r="I82">
+        <v>1950</v>
+      </c>
+      <c r="J82" s="2">
+        <f t="shared" si="100"/>
+        <v>134.48275862068965</v>
+      </c>
+      <c r="K82">
+        <v>0.6</v>
+      </c>
+      <c r="L82" s="3">
+        <v>4</v>
+      </c>
+      <c r="M82">
+        <v>16</v>
+      </c>
+      <c r="N82">
+        <f t="shared" si="101"/>
+        <v>256</v>
+      </c>
+      <c r="O82" s="1">
+        <f t="shared" si="102"/>
+        <v>7.6171875</v>
+      </c>
+      <c r="P82">
+        <f t="shared" si="103"/>
+        <v>0</v>
+      </c>
+      <c r="Q82" s="2">
+        <f t="shared" si="104"/>
+        <v>0</v>
+      </c>
+      <c r="R82" s="5">
+        <f t="shared" si="105"/>
+        <v>0</v>
+      </c>
+      <c r="S82" s="4">
+        <f t="shared" si="106"/>
+        <v>0</v>
+      </c>
+      <c r="T82" s="5">
+        <f t="shared" si="107"/>
+        <v>1.2163730780979534</v>
+      </c>
+      <c r="U82" s="5">
+        <f t="shared" si="108"/>
+        <v>0.33701657458563533</v>
+      </c>
+      <c r="V82" s="1">
+        <f t="shared" si="109"/>
+        <v>4.0320999999999998</v>
+      </c>
+      <c r="W82" s="3">
+        <f t="shared" si="110"/>
+        <v>3199.4317322992915</v>
+      </c>
+      <c r="X82" s="5">
+        <f t="shared" si="111"/>
+        <v>0.60948323426129813</v>
+      </c>
+      <c r="Y82" s="5">
+        <f t="shared" si="112"/>
+        <v>1.9035897435897438</v>
+      </c>
+      <c r="Z82">
+        <f t="shared" si="113"/>
+        <v>0.16927083333333334</v>
+      </c>
+      <c r="AA82">
+        <f t="shared" si="114"/>
+        <v>12.6953125</v>
+      </c>
+    </row>
+    <row r="83" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A83" s="8">
+        <v>37960</v>
+      </c>
+      <c r="C83">
+        <v>47</v>
+      </c>
+      <c r="E83">
+        <v>33</v>
+      </c>
+      <c r="F83">
+        <v>40</v>
+      </c>
+      <c r="H83">
+        <v>12.5</v>
+      </c>
+      <c r="I83">
+        <v>1875</v>
+      </c>
+      <c r="J83" s="2">
+        <f t="shared" si="100"/>
+        <v>150</v>
+      </c>
+      <c r="K83">
+        <v>0.6</v>
+      </c>
+      <c r="L83" s="3">
+        <v>4</v>
+      </c>
+      <c r="M83">
+        <v>30</v>
+      </c>
+      <c r="N83">
+        <f t="shared" si="101"/>
+        <v>270</v>
+      </c>
+      <c r="O83" s="1">
+        <f t="shared" si="102"/>
+        <v>6.9444444444444446</v>
+      </c>
+      <c r="P83">
+        <f t="shared" si="103"/>
+        <v>0</v>
+      </c>
+      <c r="Q83" s="2"/>
+      <c r="R83" s="5">
+        <f t="shared" si="105"/>
+        <v>0</v>
+      </c>
+      <c r="S83" s="4">
+        <f t="shared" si="106"/>
+        <v>0</v>
+      </c>
+      <c r="T83" s="5"/>
+      <c r="U83" s="5">
+        <f t="shared" si="108"/>
+        <v>0</v>
+      </c>
+      <c r="V83" s="1">
+        <f t="shared" si="109"/>
+        <v>0</v>
+      </c>
+      <c r="W83" s="3"/>
+      <c r="X83" s="5"/>
+      <c r="Y83" s="5">
+        <f t="shared" si="112"/>
+        <v>1.8</v>
+      </c>
+      <c r="Z83">
+        <f t="shared" si="113"/>
+        <v>0.14775413711583923</v>
+      </c>
+      <c r="AA83">
+        <f t="shared" si="114"/>
+        <v>11.574074074074074</v>
       </c>
     </row>
   </sheetData>

</xml_diff>